<commit_message>
Linear regression added, new sheets added to excel too
</commit_message>
<xml_diff>
--- a/New_DB.xlsx
+++ b/New_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\MCC\Thesis\Project\2024_Project\new_election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB1C31D5-5BDC-4ADF-8213-F5DF56B23D57}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{886A7E3E-154F-46BF-888F-5469B7681DAF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12567" yWindow="0" windowWidth="12568" windowHeight="13523" tabRatio="819" activeTab="4" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Galvez" sheetId="13" r:id="rId1"/>
@@ -18,6 +18,7 @@
     <sheet name="Maynez" sheetId="21" r:id="rId3"/>
     <sheet name="Accounts" sheetId="6" r:id="rId4"/>
     <sheet name="Polls" sheetId="20" r:id="rId5"/>
+    <sheet name="Vida Post" sheetId="22" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="51">
   <si>
     <t>Candidate</t>
   </si>
@@ -191,6 +192,9 @@
   <si>
     <t>Reforma</t>
   </si>
+  <si>
+    <t>Days</t>
+  </si>
 </sst>
 </file>
 
@@ -221,7 +225,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -237,6 +241,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -271,7 +281,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -306,6 +316,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -315,7 +326,10 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -637,9 +651,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6041754-B9A0-4B1F-8AE9-569EC65B3AFE}">
   <dimension ref="A1:XFB168"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A43" sqref="A43"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A110" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D134" sqref="D134"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -664,43 +678,43 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:28 16259:16382" x14ac:dyDescent="0.3">
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="15" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="14" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="14" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="14" t="s">
+      <c r="T1" s="16"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="17"/>
     </row>
     <row r="2" spans="1:28 16259:16382" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -9889,7 +9903,7 @@
   <dimension ref="A1:XFB174"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="A120" sqref="A120"/>
     </sheetView>
   </sheetViews>
@@ -9914,43 +9928,43 @@
   <sheetData>
     <row r="1" spans="1:28 16259:16382" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="15" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="14" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="14" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="14" t="s">
+      <c r="T1" s="16"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="17"/>
     </row>
     <row r="2" spans="1:28 16259:16382" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -19236,43 +19250,43 @@
   <sheetData>
     <row r="1" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A1" s="11"/>
-      <c r="B1" s="14" t="s">
+      <c r="B1" s="15" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="15"/>
-      <c r="D1" s="15"/>
-      <c r="E1" s="15"/>
-      <c r="F1" s="15"/>
-      <c r="G1" s="15"/>
-      <c r="H1" s="16"/>
-      <c r="I1" s="15" t="s">
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="17"/>
+      <c r="I1" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
-      <c r="L1" s="15"/>
-      <c r="M1" s="15"/>
-      <c r="N1" s="15"/>
-      <c r="O1" s="16"/>
-      <c r="P1" s="14" t="s">
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
+      <c r="N1" s="16"/>
+      <c r="O1" s="17"/>
+      <c r="P1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="15"/>
-      <c r="R1" s="15"/>
-      <c r="S1" s="14" t="s">
+      <c r="Q1" s="16"/>
+      <c r="R1" s="16"/>
+      <c r="S1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="15"/>
-      <c r="U1" s="16"/>
-      <c r="V1" s="14" t="s">
+      <c r="T1" s="16"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="W1" s="15"/>
-      <c r="X1" s="15"/>
-      <c r="Y1" s="15"/>
-      <c r="Z1" s="15"/>
-      <c r="AA1" s="15"/>
-      <c r="AB1" s="16"/>
+      <c r="W1" s="16"/>
+      <c r="X1" s="16"/>
+      <c r="Y1" s="16"/>
+      <c r="Z1" s="16"/>
+      <c r="AA1" s="16"/>
+      <c r="AB1" s="17"/>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -19437,7 +19451,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62C3539-067A-49FB-A3DE-0B279692F912}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
@@ -19464,7 +19478,7 @@
       <c r="A2" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="17">
+      <c r="B2" s="14">
         <v>45182</v>
       </c>
       <c r="C2">
@@ -19478,7 +19492,7 @@
       <c r="A3" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="14">
         <v>45184</v>
       </c>
       <c r="C3">
@@ -19494,7 +19508,7 @@
       <c r="A4" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="17">
+      <c r="B4" s="14">
         <v>45214</v>
       </c>
       <c r="C4">
@@ -19510,7 +19524,7 @@
       <c r="A5" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="17">
+      <c r="B5" s="14">
         <v>45214</v>
       </c>
       <c r="C5">
@@ -19526,7 +19540,7 @@
       <c r="A6" t="s">
         <v>43</v>
       </c>
-      <c r="B6" s="17">
+      <c r="B6" s="14">
         <v>45230</v>
       </c>
       <c r="C6">
@@ -19581,7 +19595,7 @@
       <c r="A10" t="s">
         <v>43</v>
       </c>
-      <c r="B10" s="17">
+      <c r="B10" s="14">
         <v>44927</v>
       </c>
       <c r="C10">
@@ -19623,7 +19637,7 @@
       <c r="A13" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="17">
+      <c r="B13" s="14">
         <v>45275</v>
       </c>
       <c r="C13">
@@ -19665,7 +19679,7 @@
       <c r="A16" t="s">
         <v>46</v>
       </c>
-      <c r="B16" s="17">
+      <c r="B16" s="14">
         <v>45265</v>
       </c>
       <c r="C16">
@@ -19680,4 +19694,407 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC47CE33-EEC3-446C-940D-05592E4B50CB}">
+  <dimension ref="A1:N32"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O12" sqref="O12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" s="18"/>
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+    </row>
+    <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3" s="19">
+        <v>1</v>
+      </c>
+      <c r="F3" s="19">
+        <v>1</v>
+      </c>
+      <c r="K3" s="19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4" s="19">
+        <v>2</v>
+      </c>
+      <c r="F4" s="19">
+        <v>2</v>
+      </c>
+      <c r="K4" s="19">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5" s="19">
+        <v>3</v>
+      </c>
+      <c r="F5" s="19">
+        <v>3</v>
+      </c>
+      <c r="K5" s="19">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6" s="19">
+        <v>4</v>
+      </c>
+      <c r="F6" s="19">
+        <v>4</v>
+      </c>
+      <c r="K6" s="19">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7" s="19">
+        <v>5</v>
+      </c>
+      <c r="F7" s="19">
+        <v>5</v>
+      </c>
+      <c r="K7" s="19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8" s="19">
+        <v>6</v>
+      </c>
+      <c r="F8" s="19">
+        <v>6</v>
+      </c>
+      <c r="K8" s="19">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9" s="19">
+        <v>7</v>
+      </c>
+      <c r="F9" s="19">
+        <v>7</v>
+      </c>
+      <c r="K9" s="19">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A10" s="19">
+        <v>8</v>
+      </c>
+      <c r="F10" s="19">
+        <v>8</v>
+      </c>
+      <c r="K10" s="19">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A11" s="19">
+        <v>9</v>
+      </c>
+      <c r="F11" s="19">
+        <v>9</v>
+      </c>
+      <c r="K11" s="19">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A12" s="19">
+        <v>10</v>
+      </c>
+      <c r="F12" s="19">
+        <v>10</v>
+      </c>
+      <c r="K12" s="19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A13" s="19">
+        <v>11</v>
+      </c>
+      <c r="F13" s="19">
+        <v>11</v>
+      </c>
+      <c r="K13" s="19">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A14" s="19">
+        <v>12</v>
+      </c>
+      <c r="F14" s="19">
+        <v>12</v>
+      </c>
+      <c r="K14" s="19">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A15" s="19">
+        <v>13</v>
+      </c>
+      <c r="F15" s="19">
+        <v>13</v>
+      </c>
+      <c r="K15" s="19">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A16" s="19">
+        <v>14</v>
+      </c>
+      <c r="F16" s="19">
+        <v>14</v>
+      </c>
+      <c r="K16" s="19">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A17" s="19">
+        <v>15</v>
+      </c>
+      <c r="F17" s="19">
+        <v>15</v>
+      </c>
+      <c r="K17" s="19">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="19">
+        <v>16</v>
+      </c>
+      <c r="F18" s="19">
+        <v>16</v>
+      </c>
+      <c r="K18" s="19">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A19" s="19">
+        <v>17</v>
+      </c>
+      <c r="F19" s="19">
+        <v>17</v>
+      </c>
+      <c r="K19" s="19">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A20" s="19">
+        <v>18</v>
+      </c>
+      <c r="F20" s="19">
+        <v>18</v>
+      </c>
+      <c r="K20" s="19">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="19">
+        <v>19</v>
+      </c>
+      <c r="F21" s="19">
+        <v>19</v>
+      </c>
+      <c r="K21" s="19">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A22" s="19">
+        <v>20</v>
+      </c>
+      <c r="F22" s="19">
+        <v>20</v>
+      </c>
+      <c r="K22" s="19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A23" s="19">
+        <v>21</v>
+      </c>
+      <c r="F23" s="19">
+        <v>21</v>
+      </c>
+      <c r="K23" s="19">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A24" s="19">
+        <v>22</v>
+      </c>
+      <c r="F24" s="19">
+        <v>22</v>
+      </c>
+      <c r="K24" s="19">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A25" s="19">
+        <v>23</v>
+      </c>
+      <c r="F25" s="19">
+        <v>23</v>
+      </c>
+      <c r="K25" s="19">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A26" s="19">
+        <v>24</v>
+      </c>
+      <c r="F26" s="19">
+        <v>24</v>
+      </c>
+      <c r="K26" s="19">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A27" s="19">
+        <v>25</v>
+      </c>
+      <c r="F27" s="19">
+        <v>25</v>
+      </c>
+      <c r="K27" s="19">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A28" s="19">
+        <v>26</v>
+      </c>
+      <c r="F28" s="19">
+        <v>26</v>
+      </c>
+      <c r="K28" s="19">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A29" s="19">
+        <v>27</v>
+      </c>
+      <c r="F29" s="19">
+        <v>27</v>
+      </c>
+      <c r="K29" s="19">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A30" s="19">
+        <v>28</v>
+      </c>
+      <c r="F30" s="19">
+        <v>28</v>
+      </c>
+      <c r="K30" s="19">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A31" s="19">
+        <v>29</v>
+      </c>
+      <c r="F31" s="19">
+        <v>29</v>
+      </c>
+      <c r="K31" s="19">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A32" s="19">
+        <v>30</v>
+      </c>
+      <c r="F32" s="19">
+        <v>30</v>
+      </c>
+      <c r="K32" s="19">
+        <v>30</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="F1:I1"/>
+    <mergeCell ref="K1:N1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
databases changed dates to consecutive date records
</commit_message>
<xml_diff>
--- a/New_DB.xlsx
+++ b/New_DB.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\MCC\Thesis\Project\2024_Project\new_election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93AAB1F5-7A86-44BF-9725-E0DFBDE13C99}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79E52567-40BF-4404-858A-73C10621D14B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" activeTab="2" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" activeTab="6" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Galvez" sheetId="13" r:id="rId1"/>
@@ -19,7 +19,7 @@
     <sheet name="Accounts" sheetId="6" r:id="rId4"/>
     <sheet name="Polls" sheetId="20" r:id="rId5"/>
     <sheet name="Vida Post" sheetId="22" r:id="rId6"/>
-    <sheet name="Means" sheetId="23" r:id="rId7"/>
+    <sheet name="Results" sheetId="23" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -64,7 +64,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="71">
   <si>
     <t>Candidate</t>
   </si>
@@ -258,40 +258,25 @@
     <t>AV</t>
   </si>
   <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>Oct</t>
-  </si>
-  <si>
-    <t>Sep</t>
-  </si>
-  <si>
-    <t>Nov</t>
-  </si>
-  <si>
-    <t>Dec</t>
-  </si>
-  <si>
-    <t>Jan</t>
-  </si>
-  <si>
-    <t>Likes in X (Daily Average)</t>
-  </si>
-  <si>
-    <t>Last Poll (%)</t>
-  </si>
-  <si>
-    <t>LR (%)</t>
-  </si>
-  <si>
-    <t>RF (%)</t>
-  </si>
-  <si>
     <t>Diff1v2</t>
   </si>
   <si>
     <t>Diff2v3</t>
+  </si>
+  <si>
+    <t>Oraculus</t>
+  </si>
+  <si>
+    <t>LR (X &amp; FB)</t>
+  </si>
+  <si>
+    <t>MLP (X &amp; FB)</t>
+  </si>
+  <si>
+    <t>LR (ALL)</t>
+  </si>
+  <si>
+    <t>MLP (AlL)</t>
   </si>
 </sst>
 </file>
@@ -446,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -515,6 +500,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -840,8 +828,8 @@
   <dimension ref="A1:XEU253"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A163" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F182" sqref="F182"/>
+      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D177" sqref="D177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -12765,15 +12753,15 @@
         <v>2727</v>
       </c>
       <c r="M163" s="6">
-        <f t="shared" ref="M163:M170" si="64">J163/I163</f>
+        <f t="shared" ref="M163:M172" si="64">J163/I163</f>
         <v>11666.666666666666</v>
       </c>
       <c r="N163" s="6">
-        <f t="shared" ref="N163:N170" si="65">K163/I163</f>
+        <f t="shared" ref="N163:N172" si="65">K163/I163</f>
         <v>2266.6666666666665</v>
       </c>
       <c r="O163" s="8">
-        <f t="shared" ref="O163:O170" si="66">L163/I163</f>
+        <f t="shared" ref="O163:O172" si="66">L163/I163</f>
         <v>909</v>
       </c>
       <c r="P163" s="6">
@@ -13033,15 +13021,15 @@
         <v>65000</v>
       </c>
       <c r="F167" s="6">
-        <f t="shared" ref="F167:F170" si="68">C167/B167</f>
+        <f t="shared" ref="F167:F172" si="68">C167/B167</f>
         <v>1966.6666666666667</v>
       </c>
       <c r="G167" s="6">
-        <f t="shared" ref="G167:G170" si="69">D167/B167</f>
+        <f t="shared" ref="G167:G172" si="69">D167/B167</f>
         <v>8100</v>
       </c>
       <c r="H167" s="8">
-        <f t="shared" ref="H167:H170" si="70">E167/B167</f>
+        <f t="shared" ref="H167:H172" si="70">E167/B167</f>
         <v>21666.666666666668</v>
       </c>
       <c r="I167" s="6">
@@ -13308,30 +13296,119 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B171" s="6"/>
-      <c r="C171" s="6"/>
-      <c r="D171" s="6"/>
-      <c r="E171" s="6"/>
-      <c r="I171" s="6"/>
-      <c r="J171" s="6"/>
-      <c r="K171" s="6"/>
-      <c r="L171" s="6"/>
+      <c r="A171" s="9">
+        <v>45344</v>
+      </c>
+      <c r="B171" s="6">
+        <v>9</v>
+      </c>
+      <c r="C171" s="6">
+        <v>12963</v>
+      </c>
+      <c r="D171" s="6">
+        <v>32829</v>
+      </c>
+      <c r="E171" s="6">
+        <v>100600</v>
+      </c>
+      <c r="F171" s="6">
+        <f t="shared" si="68"/>
+        <v>1440.3333333333333</v>
+      </c>
+      <c r="G171" s="6">
+        <f t="shared" si="69"/>
+        <v>3647.6666666666665</v>
+      </c>
+      <c r="H171" s="8">
+        <f t="shared" si="70"/>
+        <v>11177.777777777777</v>
+      </c>
+      <c r="I171" s="6">
+        <v>7</v>
+      </c>
+      <c r="J171" s="6">
+        <v>95700</v>
+      </c>
+      <c r="K171" s="6">
+        <v>19961</v>
+      </c>
+      <c r="L171" s="6">
+        <v>4129</v>
+      </c>
+      <c r="M171" s="6">
+        <f t="shared" si="64"/>
+        <v>13671.428571428571</v>
+      </c>
+      <c r="N171" s="6">
+        <f t="shared" si="65"/>
+        <v>2851.5714285714284</v>
+      </c>
+      <c r="O171" s="8">
+        <f t="shared" si="66"/>
+        <v>589.85714285714289</v>
+      </c>
       <c r="P171" s="6"/>
       <c r="Q171" s="6"/>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B172" s="6"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="6"/>
-      <c r="E172" s="6"/>
-      <c r="I172" s="6"/>
-      <c r="J172" s="6"/>
-      <c r="K172" s="6"/>
-      <c r="L172" s="6"/>
+      <c r="A172" s="9">
+        <v>45345</v>
+      </c>
+      <c r="B172" s="6">
+        <v>4</v>
+      </c>
+      <c r="C172" s="6">
+        <v>5450</v>
+      </c>
+      <c r="D172" s="6">
+        <v>22100</v>
+      </c>
+      <c r="E172" s="6">
+        <v>47000</v>
+      </c>
+      <c r="F172" s="6">
+        <f t="shared" si="68"/>
+        <v>1362.5</v>
+      </c>
+      <c r="G172" s="6">
+        <f t="shared" si="69"/>
+        <v>5525</v>
+      </c>
+      <c r="H172" s="8">
+        <f t="shared" si="70"/>
+        <v>11750</v>
+      </c>
+      <c r="I172" s="6">
+        <v>4</v>
+      </c>
+      <c r="J172" s="6">
+        <v>28800</v>
+      </c>
+      <c r="K172" s="6">
+        <v>10900</v>
+      </c>
+      <c r="L172" s="6">
+        <v>3622</v>
+      </c>
+      <c r="M172" s="6">
+        <f t="shared" si="64"/>
+        <v>7200</v>
+      </c>
+      <c r="N172" s="6">
+        <f t="shared" si="65"/>
+        <v>2725</v>
+      </c>
+      <c r="O172" s="8">
+        <f t="shared" si="66"/>
+        <v>905.5</v>
+      </c>
       <c r="P172" s="6"/>
       <c r="Q172" s="6"/>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A173" s="9">
+        <v>45346</v>
+      </c>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="6"/>
@@ -13344,6 +13421,9 @@
       <c r="Q173" s="6"/>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A174" s="9">
+        <v>45347</v>
+      </c>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
@@ -13380,11 +13460,9 @@
       <c r="Q176" s="6"/>
     </row>
     <row r="177" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B177" s="6"/>
       <c r="C177" s="6"/>
       <c r="D177" s="6"/>
       <c r="E177" s="6"/>
-      <c r="I177" s="6"/>
       <c r="J177" s="6"/>
       <c r="K177" s="6"/>
       <c r="L177" s="6"/>
@@ -13408,6 +13486,7 @@
       <c r="C179" s="6"/>
       <c r="D179" s="6"/>
       <c r="E179" s="6"/>
+      <c r="I179" s="6"/>
       <c r="J179" s="6"/>
       <c r="K179" s="6"/>
       <c r="L179" s="6"/>
@@ -13427,6 +13506,7 @@
       <c r="Q180" s="6"/>
     </row>
     <row r="181" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B181" s="6"/>
       <c r="C181" s="6"/>
       <c r="D181" s="6"/>
       <c r="E181" s="6"/>
@@ -13928,8 +14008,8 @@
   <dimension ref="A1:XET202"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A138" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E172" sqref="E172"/>
+      <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C179" sqref="C179"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -22748,15 +22828,15 @@
         <v>25700</v>
       </c>
       <c r="F121" s="6">
-        <f t="shared" ref="F121:F170" si="31">C121/B121</f>
+        <f t="shared" ref="F121:F172" si="31">C121/B121</f>
         <v>464.5</v>
       </c>
       <c r="G121" s="6">
-        <f t="shared" ref="G121:G170" si="32">D121/B121</f>
+        <f t="shared" ref="G121:G172" si="32">D121/B121</f>
         <v>894.1</v>
       </c>
       <c r="H121" s="8">
-        <f t="shared" ref="H121:H170" si="33">E121/B121</f>
+        <f t="shared" ref="H121:H172" si="33">E121/B121</f>
         <v>2570</v>
       </c>
       <c r="I121" s="6">
@@ -25757,15 +25837,15 @@
         <v>8422</v>
       </c>
       <c r="M162" s="6">
-        <f t="shared" ref="M162:M170" si="38">J162/I162</f>
+        <f t="shared" ref="M162:M172" si="38">J162/I162</f>
         <v>12650</v>
       </c>
       <c r="N162" s="6">
-        <f t="shared" ref="N162:N170" si="39">K162/I162</f>
+        <f t="shared" ref="N162:N172" si="39">K162/I162</f>
         <v>1410.8333333333333</v>
       </c>
       <c r="O162" s="8">
-        <f t="shared" ref="O162:O170" si="40">L162/I162</f>
+        <f t="shared" ref="O162:O172" si="40">L162/I162</f>
         <v>1403.6666666666667</v>
       </c>
       <c r="P162" s="6">
@@ -26372,30 +26452,119 @@
       </c>
     </row>
     <row r="171" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B171" s="6"/>
-      <c r="C171" s="6"/>
-      <c r="D171" s="6"/>
-      <c r="E171" s="6"/>
-      <c r="I171" s="6"/>
-      <c r="J171" s="6"/>
-      <c r="K171" s="6"/>
-      <c r="L171" s="6"/>
+      <c r="A171" s="9">
+        <v>45344</v>
+      </c>
+      <c r="B171" s="6">
+        <v>3</v>
+      </c>
+      <c r="C171" s="6">
+        <v>8400</v>
+      </c>
+      <c r="D171" s="6">
+        <v>11700</v>
+      </c>
+      <c r="E171" s="6">
+        <v>27500</v>
+      </c>
+      <c r="F171" s="6">
+        <f t="shared" si="31"/>
+        <v>2800</v>
+      </c>
+      <c r="G171" s="6">
+        <f t="shared" si="32"/>
+        <v>3900</v>
+      </c>
+      <c r="H171" s="8">
+        <f t="shared" si="33"/>
+        <v>9166.6666666666661</v>
+      </c>
+      <c r="I171" s="6">
+        <v>7</v>
+      </c>
+      <c r="J171" s="6">
+        <v>64000</v>
+      </c>
+      <c r="K171" s="6">
+        <v>6032</v>
+      </c>
+      <c r="L171" s="6">
+        <v>6753</v>
+      </c>
+      <c r="M171" s="6">
+        <f t="shared" si="38"/>
+        <v>9142.8571428571431</v>
+      </c>
+      <c r="N171" s="6">
+        <f t="shared" si="39"/>
+        <v>861.71428571428567</v>
+      </c>
+      <c r="O171" s="8">
+        <f t="shared" si="40"/>
+        <v>964.71428571428567</v>
+      </c>
       <c r="P171" s="6"/>
       <c r="Q171" s="6"/>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B172" s="6"/>
-      <c r="C172" s="6"/>
-      <c r="D172" s="6"/>
-      <c r="E172" s="6"/>
-      <c r="I172" s="6"/>
-      <c r="J172" s="6"/>
-      <c r="K172" s="6"/>
-      <c r="L172" s="6"/>
+      <c r="A172" s="9">
+        <v>45345</v>
+      </c>
+      <c r="B172" s="6">
+        <v>2</v>
+      </c>
+      <c r="C172" s="6">
+        <v>5700</v>
+      </c>
+      <c r="D172" s="6">
+        <v>5500</v>
+      </c>
+      <c r="E172" s="6">
+        <v>14600</v>
+      </c>
+      <c r="F172" s="6">
+        <f t="shared" si="31"/>
+        <v>2850</v>
+      </c>
+      <c r="G172" s="6">
+        <f t="shared" si="32"/>
+        <v>2750</v>
+      </c>
+      <c r="H172" s="8">
+        <f t="shared" si="33"/>
+        <v>7300</v>
+      </c>
+      <c r="I172" s="6">
+        <v>5</v>
+      </c>
+      <c r="J172" s="6">
+        <v>22600</v>
+      </c>
+      <c r="K172" s="6">
+        <v>2452</v>
+      </c>
+      <c r="L172" s="6">
+        <v>2854</v>
+      </c>
+      <c r="M172" s="6">
+        <f t="shared" si="38"/>
+        <v>4520</v>
+      </c>
+      <c r="N172" s="6">
+        <f t="shared" si="39"/>
+        <v>490.4</v>
+      </c>
+      <c r="O172" s="8">
+        <f t="shared" si="40"/>
+        <v>570.79999999999995</v>
+      </c>
       <c r="P172" s="6"/>
       <c r="Q172" s="6"/>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A173" s="9">
+        <v>45346</v>
+      </c>
       <c r="B173" s="6"/>
       <c r="C173" s="6"/>
       <c r="D173" s="6"/>
@@ -26408,6 +26577,9 @@
       <c r="Q173" s="6"/>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A174" s="9">
+        <v>45347</v>
+      </c>
       <c r="B174" s="6"/>
       <c r="C174" s="6"/>
       <c r="D174" s="6"/>
@@ -26420,7 +26592,6 @@
       <c r="Q174" s="6"/>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B175" s="6"/>
       <c r="C175" s="6"/>
       <c r="D175" s="6"/>
       <c r="E175" s="6"/>
@@ -26456,6 +26627,7 @@
       <c r="Q177" s="6"/>
     </row>
     <row r="178" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B178" s="6"/>
       <c r="C178" s="6"/>
       <c r="D178" s="6"/>
       <c r="E178" s="6"/>
@@ -26495,6 +26667,7 @@
       <c r="C181" s="6"/>
       <c r="D181" s="6"/>
       <c r="E181" s="6"/>
+      <c r="I181" s="6"/>
       <c r="J181" s="6"/>
       <c r="K181" s="6"/>
       <c r="L181" s="6"/>
@@ -26696,9 +26869,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF91097-4FB7-4052-890B-7AEB04A1F433}">
   <dimension ref="A1:V74"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E51" sqref="E51"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D50" sqref="D50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -27006,15 +27179,15 @@
         <v>321</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M44" si="4">J5/I5</f>
+        <f t="shared" ref="M5:M46" si="4">J5/I5</f>
         <v>248.5</v>
       </c>
       <c r="N5" s="6">
-        <f t="shared" ref="N5:N44" si="5">K5/I5</f>
+        <f t="shared" ref="N5:N46" si="5">K5/I5</f>
         <v>47.6</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" ref="O5:O44" si="6">L5/I5</f>
+        <f t="shared" ref="O5:O46" si="6">L5/I5</f>
         <v>32.1</v>
       </c>
       <c r="P5" s="6">
@@ -29508,15 +29681,15 @@
         <v>160</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" ref="F40:F44" si="16">C40/B40</f>
+        <f t="shared" ref="F40:F46" si="16">C40/B40</f>
         <v>904</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" ref="G40:G44" si="17">D40/B40</f>
+        <f t="shared" ref="G40:G46" si="17">D40/B40</f>
         <v>98</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" ref="H40:H44" si="18">E40/B40</f>
+        <f t="shared" ref="H40:H46" si="18">E40/B40</f>
         <v>160</v>
       </c>
       <c r="I40" s="6">
@@ -29851,30 +30024,119 @@
       </c>
     </row>
     <row r="45" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B45" s="6"/>
-      <c r="C45" s="6"/>
-      <c r="D45" s="6"/>
-      <c r="E45" s="6"/>
-      <c r="I45" s="6"/>
-      <c r="J45" s="6"/>
-      <c r="K45" s="6"/>
-      <c r="L45" s="6"/>
+      <c r="A45" s="9">
+        <v>45344</v>
+      </c>
+      <c r="B45" s="6">
+        <v>5</v>
+      </c>
+      <c r="C45" s="6">
+        <v>802</v>
+      </c>
+      <c r="D45" s="6">
+        <v>251</v>
+      </c>
+      <c r="E45" s="6">
+        <v>638</v>
+      </c>
+      <c r="F45" s="6">
+        <f t="shared" si="16"/>
+        <v>160.4</v>
+      </c>
+      <c r="G45" s="6">
+        <f t="shared" si="17"/>
+        <v>50.2</v>
+      </c>
+      <c r="H45" s="8">
+        <f t="shared" si="18"/>
+        <v>127.6</v>
+      </c>
+      <c r="I45" s="6">
+        <v>13</v>
+      </c>
+      <c r="J45" s="6">
+        <v>2896</v>
+      </c>
+      <c r="K45" s="6">
+        <v>316</v>
+      </c>
+      <c r="L45" s="6">
+        <v>389</v>
+      </c>
+      <c r="M45" s="6">
+        <f t="shared" si="4"/>
+        <v>222.76923076923077</v>
+      </c>
+      <c r="N45" s="6">
+        <f t="shared" si="5"/>
+        <v>24.307692307692307</v>
+      </c>
+      <c r="O45" s="8">
+        <f t="shared" si="6"/>
+        <v>29.923076923076923</v>
+      </c>
       <c r="P45" s="6"/>
       <c r="Q45" s="6"/>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="I46" s="6"/>
-      <c r="J46" s="6"/>
-      <c r="K46" s="6"/>
-      <c r="L46" s="6"/>
+      <c r="A46" s="9">
+        <v>45345</v>
+      </c>
+      <c r="B46" s="6">
+        <v>4</v>
+      </c>
+      <c r="C46" s="6">
+        <v>350</v>
+      </c>
+      <c r="D46" s="6">
+        <v>138</v>
+      </c>
+      <c r="E46" s="6">
+        <v>486</v>
+      </c>
+      <c r="F46" s="6">
+        <f t="shared" si="16"/>
+        <v>87.5</v>
+      </c>
+      <c r="G46" s="6">
+        <f t="shared" si="17"/>
+        <v>34.5</v>
+      </c>
+      <c r="H46" s="8">
+        <f t="shared" si="18"/>
+        <v>121.5</v>
+      </c>
+      <c r="I46" s="6">
+        <v>8</v>
+      </c>
+      <c r="J46" s="6">
+        <v>1238</v>
+      </c>
+      <c r="K46" s="6">
+        <v>183</v>
+      </c>
+      <c r="L46" s="6">
+        <v>191</v>
+      </c>
+      <c r="M46" s="6">
+        <f t="shared" si="4"/>
+        <v>154.75</v>
+      </c>
+      <c r="N46" s="6">
+        <f t="shared" si="5"/>
+        <v>22.875</v>
+      </c>
+      <c r="O46" s="8">
+        <f t="shared" si="6"/>
+        <v>23.875</v>
+      </c>
       <c r="P46" s="6"/>
       <c r="Q46" s="6"/>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A47" s="9">
+        <v>45346</v>
+      </c>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="6"/>
@@ -29887,6 +30149,10 @@
       <c r="Q47" s="6"/>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A48" s="9">
+        <v>45347</v>
+      </c>
+      <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="6"/>
       <c r="E48" s="6"/>
@@ -29898,6 +30164,10 @@
       <c r="Q48" s="6"/>
     </row>
     <row r="49" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
       <c r="I49" s="6"/>
       <c r="J49" s="6"/>
       <c r="K49" s="6"/>
@@ -29916,10 +30186,10 @@
       <c r="L50" s="6"/>
     </row>
     <row r="51" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
       <c r="E51" s="6"/>
+      <c r="I51" s="6"/>
       <c r="J51" s="6"/>
       <c r="K51" s="6"/>
       <c r="L51" s="6"/>
@@ -29967,7 +30237,6 @@
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
-      <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
@@ -30076,6 +30345,12 @@
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
       <c r="L65" s="6"/>
+    </row>
+    <row r="66" spans="9:12" x14ac:dyDescent="0.3">
+      <c r="I66" s="6"/>
+      <c r="J66" s="6"/>
+      <c r="K66" s="6"/>
+      <c r="L66" s="6"/>
     </row>
     <row r="67" spans="9:12" x14ac:dyDescent="0.3">
       <c r="I67" s="6"/>
@@ -30141,7 +30416,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -30246,10 +30521,10 @@
         <v>52</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="I1" s="1" t="s">
         <v>62</v>
@@ -32055,120 +32330,75 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6748DF8D-1E96-42F5-BE18-DD686141E658}">
-  <dimension ref="A2:M6"/>
+  <dimension ref="B2:M7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I2" s="6"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
+      <c r="M2" s="6"/>
+    </row>
+    <row r="3" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I3" s="6"/>
+      <c r="J3" s="6"/>
+      <c r="K3" s="6"/>
+      <c r="L3" s="6"/>
+      <c r="M3" s="6"/>
+    </row>
+    <row r="4" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="I4" s="6"/>
+      <c r="J4" s="6"/>
+      <c r="K4" s="6"/>
+      <c r="L4" s="6"/>
+      <c r="M4" s="6"/>
+    </row>
+    <row r="5" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="C5" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="I2" s="6"/>
-      <c r="J2" s="6" t="s">
-        <v>71</v>
-      </c>
-      <c r="K2" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="L2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="M2" s="6"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B3" t="s">
-        <v>66</v>
-      </c>
-      <c r="C3" t="s">
-        <v>65</v>
-      </c>
-      <c r="D3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" t="s">
-        <v>68</v>
-      </c>
-      <c r="F3" t="s">
-        <v>69</v>
-      </c>
-      <c r="I3" s="6" t="s">
+    </row>
+    <row r="6" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B6" t="s">
         <v>61</v>
       </c>
-      <c r="J3" s="6">
-        <v>63</v>
-      </c>
-      <c r="K3" s="6">
-        <v>55</v>
-      </c>
-      <c r="L3" s="6">
-        <v>54</v>
-      </c>
-      <c r="M3" s="6"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>51</v>
-      </c>
-      <c r="B4">
-        <v>33426</v>
-      </c>
-      <c r="C4">
-        <v>18143</v>
-      </c>
-      <c r="D4">
-        <v>24328</v>
-      </c>
-      <c r="E4">
-        <v>24617</v>
-      </c>
-      <c r="F4">
-        <v>22640</v>
-      </c>
-      <c r="I4" s="6" t="s">
+      <c r="C6" s="30">
+        <v>0.64</v>
+      </c>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+    </row>
+    <row r="7" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="B7" t="s">
         <v>3</v>
       </c>
-      <c r="J4" s="6">
-        <v>22</v>
-      </c>
-      <c r="K4" s="6">
-        <v>25</v>
-      </c>
-      <c r="L4" s="6">
-        <v>25</v>
-      </c>
-      <c r="M4" s="6"/>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>50</v>
-      </c>
-      <c r="B5">
-        <v>51000</v>
-      </c>
-      <c r="C5">
-        <v>40000</v>
-      </c>
-      <c r="D5">
-        <v>55792</v>
-      </c>
-      <c r="E5">
-        <v>43850</v>
-      </c>
-      <c r="F5">
-        <v>68864</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>64</v>
-      </c>
+      <c r="C7" s="30">
+        <v>0.3</v>
+      </c>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
MLP created and evaluated
</commit_message>
<xml_diff>
--- a/New_DB.xlsx
+++ b/New_DB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\MCC\Thesis\Project\2024_Project\new_election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CA772D-494B-444E-8192-B490C3DFFCA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F5C9092D-D4D4-4DCB-9A4D-A5707E2C270A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" activeTab="6" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
+    <workbookView xWindow="12567" yWindow="0" windowWidth="12568" windowHeight="13523" tabRatio="819" activeTab="2" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Galvez" sheetId="13" r:id="rId1"/>
@@ -431,7 +431,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -503,6 +503,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -828,8 +831,8 @@
   <dimension ref="A1:XEU253"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A166" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D180" sqref="D180"/>
+      <pane ySplit="1" topLeftCell="A172" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A177" sqref="A177"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -11323,7 +11326,7 @@
         <v>20269</v>
       </c>
       <c r="R143" s="8">
-        <f t="shared" ref="R143:R174" si="59">Q143/P143</f>
+        <f t="shared" ref="R143:R176" si="59">Q143/P143</f>
         <v>6756.333333333333</v>
       </c>
       <c r="S143" s="6">
@@ -12753,15 +12756,15 @@
         <v>2727</v>
       </c>
       <c r="M163" s="6">
-        <f t="shared" ref="M163:M174" si="64">J163/I163</f>
+        <f t="shared" ref="M163:M176" si="64">J163/I163</f>
         <v>11666.666666666666</v>
       </c>
       <c r="N163" s="6">
-        <f t="shared" ref="N163:N174" si="65">K163/I163</f>
+        <f t="shared" ref="N163:N176" si="65">K163/I163</f>
         <v>2266.6666666666665</v>
       </c>
       <c r="O163" s="8">
-        <f t="shared" ref="O163:O174" si="66">L163/I163</f>
+        <f t="shared" ref="O163:O176" si="66">L163/I163</f>
         <v>909</v>
       </c>
       <c r="P163" s="6">
@@ -13021,15 +13024,15 @@
         <v>65000</v>
       </c>
       <c r="F167" s="6">
-        <f t="shared" ref="F167:F174" si="68">C167/B167</f>
+        <f t="shared" ref="F167:F176" si="68">C167/B167</f>
         <v>1966.6666666666667</v>
       </c>
       <c r="G167" s="6">
-        <f t="shared" ref="G167:G174" si="69">D167/B167</f>
+        <f t="shared" ref="G167:G176" si="69">D167/B167</f>
         <v>8100</v>
       </c>
       <c r="H167" s="8">
-        <f t="shared" ref="H167:H174" si="70">E167/B167</f>
+        <f t="shared" ref="H167:H176" si="70">E167/B167</f>
         <v>21666.666666666668</v>
       </c>
       <c r="I167" s="6">
@@ -13357,6 +13360,16 @@
         <f t="shared" si="59"/>
         <v>11944.666666666666</v>
       </c>
+      <c r="S171" s="6">
+        <v>1</v>
+      </c>
+      <c r="T171" s="6">
+        <v>11000</v>
+      </c>
+      <c r="U171" s="8">
+        <f t="shared" ref="U171:U176" si="71">T171/S171</f>
+        <v>11000</v>
+      </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A172" s="9">
@@ -13420,6 +13433,16 @@
         <f t="shared" si="59"/>
         <v>10902</v>
       </c>
+      <c r="S172" s="6">
+        <v>1</v>
+      </c>
+      <c r="T172" s="6">
+        <v>9900</v>
+      </c>
+      <c r="U172" s="8">
+        <f t="shared" si="71"/>
+        <v>9900</v>
+      </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A173" s="9">
@@ -13483,6 +13506,16 @@
         <f t="shared" si="59"/>
         <v>11234.857142857143</v>
       </c>
+      <c r="S173" s="6">
+        <v>2</v>
+      </c>
+      <c r="T173" s="6">
+        <v>90000</v>
+      </c>
+      <c r="U173" s="8">
+        <f t="shared" si="71"/>
+        <v>45000</v>
+      </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A174" s="9">
@@ -13546,36 +13579,161 @@
         <f t="shared" si="59"/>
         <v>19342.333333333332</v>
       </c>
+      <c r="S174" s="6">
+        <v>2</v>
+      </c>
+      <c r="T174" s="6">
+        <v>168000</v>
+      </c>
+      <c r="U174" s="8">
+        <f t="shared" si="71"/>
+        <v>84000</v>
+      </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A175" s="9">
         <v>45348</v>
       </c>
-      <c r="B175" s="6"/>
-      <c r="C175" s="6"/>
-      <c r="D175" s="6"/>
-      <c r="E175" s="6"/>
-      <c r="I175" s="6"/>
-      <c r="J175" s="6"/>
-      <c r="K175" s="6"/>
-      <c r="L175" s="6"/>
-      <c r="P175" s="6"/>
-      <c r="Q175" s="6"/>
+      <c r="B175" s="6">
+        <v>5</v>
+      </c>
+      <c r="C175" s="6">
+        <v>6874</v>
+      </c>
+      <c r="D175" s="6">
+        <v>19600</v>
+      </c>
+      <c r="E175" s="6">
+        <v>45800</v>
+      </c>
+      <c r="F175" s="6">
+        <f t="shared" si="68"/>
+        <v>1374.8</v>
+      </c>
+      <c r="G175" s="6">
+        <f t="shared" si="69"/>
+        <v>3920</v>
+      </c>
+      <c r="H175" s="8">
+        <f t="shared" si="70"/>
+        <v>9160</v>
+      </c>
+      <c r="I175" s="6">
+        <v>5</v>
+      </c>
+      <c r="J175" s="6">
+        <v>39400</v>
+      </c>
+      <c r="K175" s="6">
+        <v>12000</v>
+      </c>
+      <c r="L175" s="6">
+        <v>3966</v>
+      </c>
+      <c r="M175" s="6">
+        <f t="shared" si="64"/>
+        <v>7880</v>
+      </c>
+      <c r="N175" s="6">
+        <f t="shared" si="65"/>
+        <v>2400</v>
+      </c>
+      <c r="O175" s="8">
+        <f t="shared" si="66"/>
+        <v>793.2</v>
+      </c>
+      <c r="P175" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q175" s="6">
+        <v>39559</v>
+      </c>
+      <c r="R175" s="8">
+        <f t="shared" si="59"/>
+        <v>9889.75</v>
+      </c>
+      <c r="S175" s="6">
+        <v>3</v>
+      </c>
+      <c r="T175" s="6">
+        <v>61100</v>
+      </c>
+      <c r="U175" s="8">
+        <f t="shared" si="71"/>
+        <v>20366.666666666668</v>
+      </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A176" s="9">
         <v>45349</v>
       </c>
-      <c r="B176" s="6"/>
-      <c r="C176" s="6"/>
-      <c r="D176" s="6"/>
-      <c r="E176" s="6"/>
-      <c r="I176" s="6"/>
-      <c r="J176" s="6"/>
-      <c r="K176" s="6"/>
-      <c r="L176" s="6"/>
-      <c r="P176" s="6"/>
-      <c r="Q176" s="6"/>
+      <c r="B176" s="6">
+        <v>5</v>
+      </c>
+      <c r="C176" s="6">
+        <v>6837</v>
+      </c>
+      <c r="D176" s="6">
+        <v>29400</v>
+      </c>
+      <c r="E176" s="6">
+        <v>67100</v>
+      </c>
+      <c r="F176" s="6">
+        <f t="shared" si="68"/>
+        <v>1367.4</v>
+      </c>
+      <c r="G176" s="6">
+        <f t="shared" si="69"/>
+        <v>5880</v>
+      </c>
+      <c r="H176" s="8">
+        <f t="shared" si="70"/>
+        <v>13420</v>
+      </c>
+      <c r="I176" s="6">
+        <v>3</v>
+      </c>
+      <c r="J176" s="6">
+        <v>20600</v>
+      </c>
+      <c r="K176" s="6">
+        <v>5400</v>
+      </c>
+      <c r="L176" s="6">
+        <v>2043</v>
+      </c>
+      <c r="M176" s="6">
+        <f t="shared" si="64"/>
+        <v>6866.666666666667</v>
+      </c>
+      <c r="N176" s="6">
+        <f t="shared" si="65"/>
+        <v>1800</v>
+      </c>
+      <c r="O176" s="8">
+        <f t="shared" si="66"/>
+        <v>681</v>
+      </c>
+      <c r="P176" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q176" s="6">
+        <v>43145</v>
+      </c>
+      <c r="R176" s="8">
+        <f t="shared" si="59"/>
+        <v>14381.666666666666</v>
+      </c>
+      <c r="S176" s="31">
+        <v>0</v>
+      </c>
+      <c r="T176" s="31">
+        <v>0</v>
+      </c>
+      <c r="U176" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="177" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B177" s="6"/>
@@ -13602,9 +13760,11 @@
       <c r="Q178" s="6"/>
     </row>
     <row r="179" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B179" s="6"/>
       <c r="C179" s="6"/>
       <c r="D179" s="6"/>
       <c r="E179" s="6"/>
+      <c r="I179" s="6"/>
       <c r="J179" s="6"/>
       <c r="K179" s="6"/>
       <c r="L179" s="6"/>
@@ -13616,7 +13776,6 @@
       <c r="C180" s="6"/>
       <c r="D180" s="6"/>
       <c r="E180" s="6"/>
-      <c r="I180" s="6"/>
       <c r="J180" s="6"/>
       <c r="K180" s="6"/>
       <c r="L180" s="6"/>
@@ -13632,9 +13791,9 @@
       <c r="J181" s="6"/>
       <c r="K181" s="6"/>
       <c r="L181" s="6"/>
+      <c r="P181" s="6"/>
     </row>
     <row r="182" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B182" s="6"/>
       <c r="C182" s="6"/>
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
@@ -14139,9 +14298,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC4418A-3538-4357-9158-8F79507C1D9F}">
   <dimension ref="A1:XET202"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="K1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A168" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C179" sqref="C179"/>
+      <selection pane="bottomLeft" activeCell="T184" sqref="T184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -22960,15 +23119,15 @@
         <v>25700</v>
       </c>
       <c r="F121" s="6">
-        <f t="shared" ref="F121:F174" si="31">C121/B121</f>
+        <f t="shared" ref="F121:F176" si="31">C121/B121</f>
         <v>464.5</v>
       </c>
       <c r="G121" s="6">
-        <f t="shared" ref="G121:G174" si="32">D121/B121</f>
+        <f t="shared" ref="G121:G176" si="32">D121/B121</f>
         <v>894.1</v>
       </c>
       <c r="H121" s="8">
-        <f t="shared" ref="H121:H174" si="33">E121/B121</f>
+        <f t="shared" ref="H121:H176" si="33">E121/B121</f>
         <v>2570</v>
       </c>
       <c r="I121" s="6">
@@ -25969,15 +26128,15 @@
         <v>8422</v>
       </c>
       <c r="M162" s="6">
-        <f t="shared" ref="M162:M174" si="38">J162/I162</f>
+        <f t="shared" ref="M162:M176" si="38">J162/I162</f>
         <v>12650</v>
       </c>
       <c r="N162" s="6">
-        <f t="shared" ref="N162:N174" si="39">K162/I162</f>
+        <f t="shared" ref="N162:N176" si="39">K162/I162</f>
         <v>1410.8333333333333</v>
       </c>
       <c r="O162" s="8">
-        <f t="shared" ref="O162:O174" si="40">L162/I162</f>
+        <f t="shared" ref="O162:O176" si="40">L162/I162</f>
         <v>1403.6666666666667</v>
       </c>
       <c r="P162" s="6">
@@ -26287,7 +26446,7 @@
         <v>33048</v>
       </c>
       <c r="U166" s="8">
-        <f t="shared" ref="U166:U170" si="41">T166/S166</f>
+        <f t="shared" ref="U166:U176" si="41">T166/S166</f>
         <v>11016</v>
       </c>
     </row>
@@ -26350,7 +26509,7 @@
         <v>74697</v>
       </c>
       <c r="R167" s="8">
-        <f t="shared" ref="R167:R174" si="42">Q167/P167</f>
+        <f t="shared" ref="R167:R176" si="42">Q167/P167</f>
         <v>10671</v>
       </c>
       <c r="S167" s="6">
@@ -26645,6 +26804,15 @@
         <f t="shared" si="42"/>
         <v>13829.75</v>
       </c>
+      <c r="S171" s="6">
+        <v>0</v>
+      </c>
+      <c r="T171" s="6">
+        <v>0</v>
+      </c>
+      <c r="U171" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="172" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A172" s="9">
@@ -26708,6 +26876,16 @@
         <f t="shared" si="42"/>
         <v>4917.5</v>
       </c>
+      <c r="S172" s="6">
+        <v>2</v>
+      </c>
+      <c r="T172" s="6">
+        <v>420000</v>
+      </c>
+      <c r="U172" s="8">
+        <f t="shared" si="41"/>
+        <v>210000</v>
+      </c>
     </row>
     <row r="173" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A173" s="9">
@@ -26771,6 +26949,15 @@
         <f t="shared" si="42"/>
         <v>7248</v>
       </c>
+      <c r="S173" s="6">
+        <v>0</v>
+      </c>
+      <c r="T173" s="6">
+        <v>0</v>
+      </c>
+      <c r="U173" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="174" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A174" s="9">
@@ -26834,36 +27021,162 @@
         <f t="shared" si="42"/>
         <v>11113.5</v>
       </c>
+      <c r="S174" s="6">
+        <v>1</v>
+      </c>
+      <c r="T174" s="6">
+        <v>27000</v>
+      </c>
+      <c r="U174" s="8">
+        <f>T174/S174</f>
+        <v>27000</v>
+      </c>
     </row>
     <row r="175" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A175" s="9">
         <v>45348</v>
       </c>
-      <c r="B175" s="6"/>
-      <c r="C175" s="6"/>
-      <c r="D175" s="6"/>
-      <c r="E175" s="6"/>
-      <c r="I175" s="6"/>
-      <c r="J175" s="6"/>
-      <c r="K175" s="6"/>
-      <c r="L175" s="6"/>
-      <c r="P175" s="6"/>
-      <c r="Q175" s="6"/>
+      <c r="B175" s="6">
+        <v>7</v>
+      </c>
+      <c r="C175" s="6">
+        <v>6432</v>
+      </c>
+      <c r="D175" s="6">
+        <v>11952</v>
+      </c>
+      <c r="E175" s="6">
+        <v>29300</v>
+      </c>
+      <c r="F175" s="6">
+        <f t="shared" si="31"/>
+        <v>918.85714285714289</v>
+      </c>
+      <c r="G175" s="6">
+        <f t="shared" si="32"/>
+        <v>1707.4285714285713</v>
+      </c>
+      <c r="H175" s="8">
+        <f t="shared" si="33"/>
+        <v>4185.7142857142853</v>
+      </c>
+      <c r="I175" s="6">
+        <v>7</v>
+      </c>
+      <c r="J175" s="6">
+        <v>39600</v>
+      </c>
+      <c r="K175" s="6">
+        <v>3800</v>
+      </c>
+      <c r="L175" s="6">
+        <v>4862</v>
+      </c>
+      <c r="M175" s="6">
+        <f t="shared" si="38"/>
+        <v>5657.1428571428569</v>
+      </c>
+      <c r="N175" s="6">
+        <f t="shared" si="39"/>
+        <v>542.85714285714289</v>
+      </c>
+      <c r="O175" s="8">
+        <f t="shared" si="40"/>
+        <v>694.57142857142856</v>
+      </c>
+      <c r="P175" s="6">
+        <v>3</v>
+      </c>
+      <c r="Q175" s="6">
+        <v>22764</v>
+      </c>
+      <c r="R175" s="8">
+        <f t="shared" si="42"/>
+        <v>7588</v>
+      </c>
+      <c r="S175" s="6">
+        <v>4</v>
+      </c>
+      <c r="T175" s="6">
+        <v>280200</v>
+      </c>
+      <c r="U175" s="8">
+        <f t="shared" si="41"/>
+        <v>70050</v>
+      </c>
     </row>
     <row r="176" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A176" s="9">
         <v>45349</v>
       </c>
-      <c r="B176" s="6"/>
-      <c r="C176" s="6"/>
-      <c r="D176" s="6"/>
-      <c r="E176" s="6"/>
-      <c r="I176" s="6"/>
-      <c r="J176" s="6"/>
-      <c r="K176" s="6"/>
-      <c r="L176" s="6"/>
-      <c r="P176" s="6"/>
-      <c r="Q176" s="6"/>
+      <c r="B176" s="6">
+        <v>6</v>
+      </c>
+      <c r="C176" s="6">
+        <v>8063</v>
+      </c>
+      <c r="D176" s="6">
+        <v>11600</v>
+      </c>
+      <c r="E176" s="6">
+        <v>32500</v>
+      </c>
+      <c r="F176" s="6">
+        <f t="shared" si="31"/>
+        <v>1343.8333333333333</v>
+      </c>
+      <c r="G176" s="6">
+        <f t="shared" si="32"/>
+        <v>1933.3333333333333</v>
+      </c>
+      <c r="H176" s="8">
+        <f t="shared" si="33"/>
+        <v>5416.666666666667</v>
+      </c>
+      <c r="I176" s="6">
+        <v>8</v>
+      </c>
+      <c r="J176" s="6">
+        <v>53300</v>
+      </c>
+      <c r="K176" s="6">
+        <v>4982</v>
+      </c>
+      <c r="L176" s="6">
+        <v>4583</v>
+      </c>
+      <c r="M176" s="6">
+        <f t="shared" si="38"/>
+        <v>6662.5</v>
+      </c>
+      <c r="N176" s="6">
+        <f t="shared" si="39"/>
+        <v>622.75</v>
+      </c>
+      <c r="O176" s="8">
+        <f t="shared" si="40"/>
+        <v>572.875</v>
+      </c>
+      <c r="P176" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q176" s="6">
+        <v>30097</v>
+      </c>
+      <c r="R176" s="8">
+        <f t="shared" si="42"/>
+        <v>6019.4</v>
+      </c>
+      <c r="S176" s="6">
+        <v>3</v>
+      </c>
+      <c r="T176" s="6">
+        <v>2406900</v>
+      </c>
+      <c r="U176" s="8">
+        <f t="shared" si="41"/>
+        <v>802300</v>
+      </c>
     </row>
     <row r="177" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B177" s="6"/>
@@ -26930,6 +27243,7 @@
       <c r="C182" s="6"/>
       <c r="D182" s="6"/>
       <c r="E182" s="6"/>
+      <c r="I182" s="6"/>
       <c r="J182" s="6"/>
       <c r="K182" s="6"/>
       <c r="L182" s="6"/>
@@ -26937,7 +27251,6 @@
       <c r="Q182" s="6"/>
     </row>
     <row r="183" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B183" s="6"/>
       <c r="C183" s="6"/>
       <c r="D183" s="6"/>
       <c r="E183" s="6"/>
@@ -27033,6 +27346,7 @@
       <c r="Q190" s="6"/>
     </row>
     <row r="191" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B191" s="6"/>
       <c r="I191" s="6"/>
       <c r="J191" s="6"/>
       <c r="K191" s="6"/>
@@ -27119,9 +27433,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF91097-4FB7-4052-890B-7AEB04A1F433}">
   <dimension ref="A1:V89"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E53" sqref="E53"/>
+    <sheetView tabSelected="1" topLeftCell="N1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A43" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T51" sqref="T51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -27429,15 +27743,15 @@
         <v>321</v>
       </c>
       <c r="M5" s="6">
-        <f t="shared" ref="M5:M48" si="4">J5/I5</f>
+        <f t="shared" ref="M5:M50" si="4">J5/I5</f>
         <v>248.5</v>
       </c>
       <c r="N5" s="6">
-        <f t="shared" ref="N5:N48" si="5">K5/I5</f>
+        <f t="shared" ref="N5:N50" si="5">K5/I5</f>
         <v>47.6</v>
       </c>
       <c r="O5" s="8">
-        <f t="shared" ref="O5:O48" si="6">L5/I5</f>
+        <f t="shared" ref="O5:O50" si="6">L5/I5</f>
         <v>32.1</v>
       </c>
       <c r="P5" s="6">
@@ -28755,7 +29069,7 @@
         <v>8328</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" ref="R23:R48" si="12">Q23/P23</f>
+        <f t="shared" ref="R23:R50" si="12">Q23/P23</f>
         <v>1189.7142857142858</v>
       </c>
       <c r="S23" s="6">
@@ -29931,15 +30245,15 @@
         <v>160</v>
       </c>
       <c r="F40" s="6">
-        <f t="shared" ref="F40:F48" si="16">C40/B40</f>
+        <f t="shared" ref="F40:F50" si="16">C40/B40</f>
         <v>904</v>
       </c>
       <c r="G40" s="6">
-        <f t="shared" ref="G40:G48" si="17">D40/B40</f>
+        <f t="shared" ref="G40:G50" si="17">D40/B40</f>
         <v>98</v>
       </c>
       <c r="H40" s="8">
-        <f t="shared" ref="H40:H48" si="18">E40/B40</f>
+        <f t="shared" ref="H40:H50" si="18">E40/B40</f>
         <v>160</v>
       </c>
       <c r="I40" s="6">
@@ -30335,6 +30649,16 @@
         <f t="shared" si="12"/>
         <v>970.36363636363637</v>
       </c>
+      <c r="S45" s="6">
+        <v>1</v>
+      </c>
+      <c r="T45" s="6">
+        <v>2400</v>
+      </c>
+      <c r="U45" s="8">
+        <f>T45/S45</f>
+        <v>2400</v>
+      </c>
     </row>
     <row r="46" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A46" s="9">
@@ -30398,6 +30722,15 @@
         <f t="shared" si="12"/>
         <v>950.7</v>
       </c>
+      <c r="S46" s="6">
+        <v>0</v>
+      </c>
+      <c r="T46" s="6">
+        <v>0</v>
+      </c>
+      <c r="U46" s="8">
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A47" s="9">
@@ -30461,6 +30794,16 @@
         <f t="shared" si="12"/>
         <v>584</v>
       </c>
+      <c r="S47" s="6">
+        <v>1</v>
+      </c>
+      <c r="T47" s="6">
+        <v>612</v>
+      </c>
+      <c r="U47" s="8">
+        <f t="shared" ref="U46:U50" si="19">T47/S47</f>
+        <v>612</v>
+      </c>
     </row>
     <row r="48" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A48" s="9">
@@ -30524,36 +30867,162 @@
         <f t="shared" si="12"/>
         <v>517.57142857142856</v>
       </c>
-    </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="S48" s="6">
+        <v>1</v>
+      </c>
+      <c r="T48" s="6">
+        <v>373</v>
+      </c>
+      <c r="U48" s="8">
+        <f t="shared" si="19"/>
+        <v>373</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A49" s="9">
         <v>45348</v>
       </c>
-      <c r="B49" s="6"/>
-      <c r="C49" s="6"/>
-      <c r="D49" s="6"/>
-      <c r="E49" s="6"/>
-      <c r="I49" s="6"/>
-      <c r="J49" s="6"/>
-      <c r="K49" s="6"/>
-      <c r="L49" s="6"/>
-      <c r="P49" s="6"/>
-      <c r="Q49" s="6"/>
-    </row>
-    <row r="50" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B49" s="6">
+        <v>5</v>
+      </c>
+      <c r="C49" s="6">
+        <v>1574</v>
+      </c>
+      <c r="D49" s="6">
+        <v>480</v>
+      </c>
+      <c r="E49" s="6">
+        <v>802</v>
+      </c>
+      <c r="F49" s="6">
+        <f t="shared" si="16"/>
+        <v>314.8</v>
+      </c>
+      <c r="G49" s="6">
+        <f t="shared" si="17"/>
+        <v>96</v>
+      </c>
+      <c r="H49" s="8">
+        <f t="shared" si="18"/>
+        <v>160.4</v>
+      </c>
+      <c r="I49" s="6">
+        <v>4</v>
+      </c>
+      <c r="J49" s="6">
+        <v>578</v>
+      </c>
+      <c r="K49" s="6">
+        <v>50</v>
+      </c>
+      <c r="L49" s="6">
+        <v>105</v>
+      </c>
+      <c r="M49" s="6">
+        <f t="shared" si="4"/>
+        <v>144.5</v>
+      </c>
+      <c r="N49" s="6">
+        <f t="shared" si="5"/>
+        <v>12.5</v>
+      </c>
+      <c r="O49" s="8">
+        <f t="shared" si="6"/>
+        <v>26.25</v>
+      </c>
+      <c r="P49" s="6">
+        <v>4</v>
+      </c>
+      <c r="Q49" s="6">
+        <v>3588</v>
+      </c>
+      <c r="R49" s="8">
+        <f t="shared" si="12"/>
+        <v>897</v>
+      </c>
+      <c r="S49" s="6">
+        <v>0</v>
+      </c>
+      <c r="T49" s="6">
+        <v>0</v>
+      </c>
+      <c r="U49" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A50" s="9">
         <v>45349</v>
       </c>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="I50" s="6"/>
-      <c r="J50" s="6"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-    </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="B50" s="6">
+        <v>11</v>
+      </c>
+      <c r="C50" s="6">
+        <v>701</v>
+      </c>
+      <c r="D50" s="6">
+        <v>294</v>
+      </c>
+      <c r="E50" s="6">
+        <v>1000</v>
+      </c>
+      <c r="F50" s="6">
+        <f t="shared" si="16"/>
+        <v>63.727272727272727</v>
+      </c>
+      <c r="G50" s="6">
+        <f t="shared" si="17"/>
+        <v>26.727272727272727</v>
+      </c>
+      <c r="H50" s="8">
+        <f t="shared" si="18"/>
+        <v>90.909090909090907</v>
+      </c>
+      <c r="I50" s="6">
+        <v>8</v>
+      </c>
+      <c r="J50" s="6">
+        <v>2131</v>
+      </c>
+      <c r="K50" s="6">
+        <v>430</v>
+      </c>
+      <c r="L50" s="6">
+        <v>217</v>
+      </c>
+      <c r="M50" s="6">
+        <f t="shared" si="4"/>
+        <v>266.375</v>
+      </c>
+      <c r="N50" s="6">
+        <f t="shared" si="5"/>
+        <v>53.75</v>
+      </c>
+      <c r="O50" s="8">
+        <f t="shared" si="6"/>
+        <v>27.125</v>
+      </c>
+      <c r="P50" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q50" s="6">
+        <v>2910</v>
+      </c>
+      <c r="R50" s="8">
+        <f t="shared" si="12"/>
+        <v>582</v>
+      </c>
+      <c r="S50" s="6">
+        <v>0</v>
+      </c>
+      <c r="T50" s="6">
+        <v>0</v>
+      </c>
+      <c r="U50" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="6"/>
@@ -30565,7 +31034,7 @@
       <c r="P51" s="6"/>
       <c r="Q51" s="6"/>
     </row>
-    <row r="52" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B52" s="6"/>
       <c r="C52" s="6"/>
       <c r="D52" s="6"/>
@@ -30577,7 +31046,7 @@
       <c r="P52" s="6"/>
       <c r="Q52" s="6"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B53" s="6"/>
       <c r="C53" s="6"/>
       <c r="D53" s="6"/>
@@ -30589,7 +31058,7 @@
       <c r="P53" s="6"/>
       <c r="Q53" s="6"/>
     </row>
-    <row r="54" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B54" s="6"/>
       <c r="C54" s="6"/>
       <c r="D54" s="6"/>
@@ -30601,17 +31070,19 @@
       <c r="P54" s="6"/>
       <c r="Q54" s="6"/>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B55" s="6"/>
       <c r="C55" s="6"/>
       <c r="D55" s="6"/>
       <c r="E55" s="6"/>
+      <c r="I55" s="6"/>
       <c r="J55" s="6"/>
       <c r="K55" s="6"/>
       <c r="L55" s="6"/>
       <c r="P55" s="6"/>
       <c r="Q55" s="6"/>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B56" s="6"/>
       <c r="C56" s="6"/>
       <c r="D56" s="6"/>
@@ -30623,7 +31094,7 @@
       <c r="P56" s="6"/>
       <c r="Q56" s="6"/>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B57" s="6"/>
       <c r="C57" s="6"/>
       <c r="D57" s="6"/>
@@ -30635,7 +31106,7 @@
       <c r="P57" s="6"/>
       <c r="Q57" s="6"/>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B58" s="6"/>
       <c r="C58" s="6"/>
       <c r="D58" s="6"/>
@@ -30647,19 +31118,18 @@
       <c r="P58" s="6"/>
       <c r="Q58" s="6"/>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B59" s="6"/>
       <c r="C59" s="6"/>
       <c r="D59" s="6"/>
       <c r="E59" s="6"/>
-      <c r="I59" s="6"/>
       <c r="J59" s="6"/>
       <c r="K59" s="6"/>
       <c r="L59" s="6"/>
       <c r="P59" s="6"/>
       <c r="Q59" s="6"/>
     </row>
-    <row r="60" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B60" s="6"/>
       <c r="C60" s="6"/>
       <c r="D60" s="6"/>
@@ -30669,8 +31139,9 @@
       <c r="K60" s="6"/>
       <c r="L60" s="6"/>
       <c r="P60" s="6"/>
-    </row>
-    <row r="61" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="Q60" s="6"/>
+    </row>
+    <row r="61" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B61" s="6"/>
       <c r="C61" s="6"/>
       <c r="D61" s="6"/>
@@ -30682,8 +31153,7 @@
       <c r="P61" s="6"/>
       <c r="Q61" s="6"/>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.3">
-      <c r="B62" s="6"/>
+    <row r="62" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C62" s="6"/>
       <c r="D62" s="6"/>
       <c r="E62" s="6"/>
@@ -30694,7 +31164,7 @@
       <c r="P62" s="6"/>
       <c r="Q62" s="6"/>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B63" s="6"/>
       <c r="C63" s="6"/>
       <c r="D63" s="6"/>
@@ -30706,7 +31176,7 @@
       <c r="P63" s="6"/>
       <c r="Q63" s="6"/>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B64" s="6"/>
       <c r="C64" s="6"/>
       <c r="D64" s="6"/>
@@ -30718,7 +31188,11 @@
       <c r="P64" s="6"/>
       <c r="Q64" s="6"/>
     </row>
-    <row r="65" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B65" s="6"/>
+      <c r="C65" s="6"/>
+      <c r="D65" s="6"/>
+      <c r="E65" s="6"/>
       <c r="I65" s="6"/>
       <c r="J65" s="6"/>
       <c r="K65" s="6"/>
@@ -30726,7 +31200,11 @@
       <c r="P65" s="6"/>
       <c r="Q65" s="6"/>
     </row>
-    <row r="66" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B66" s="6"/>
+      <c r="C66" s="6"/>
+      <c r="D66" s="6"/>
+      <c r="E66" s="6"/>
       <c r="I66" s="6"/>
       <c r="J66" s="6"/>
       <c r="K66" s="6"/>
@@ -30734,7 +31212,11 @@
       <c r="P66" s="6"/>
       <c r="Q66" s="6"/>
     </row>
-    <row r="67" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B67" s="6"/>
+      <c r="C67" s="6"/>
+      <c r="D67" s="6"/>
+      <c r="E67" s="6"/>
       <c r="I67" s="6"/>
       <c r="J67" s="6"/>
       <c r="K67" s="6"/>
@@ -30742,7 +31224,7 @@
       <c r="P67" s="6"/>
       <c r="Q67" s="6"/>
     </row>
-    <row r="68" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I68" s="6"/>
       <c r="J68" s="6"/>
       <c r="K68" s="6"/>
@@ -30750,7 +31232,7 @@
       <c r="P68" s="6"/>
       <c r="Q68" s="6"/>
     </row>
-    <row r="69" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I69" s="6"/>
       <c r="J69" s="6"/>
       <c r="K69" s="6"/>
@@ -30758,7 +31240,7 @@
       <c r="P69" s="6"/>
       <c r="Q69" s="6"/>
     </row>
-    <row r="70" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I70" s="6"/>
       <c r="J70" s="6"/>
       <c r="K70" s="6"/>
@@ -30766,14 +31248,14 @@
       <c r="P70" s="6"/>
       <c r="Q70" s="6"/>
     </row>
-    <row r="71" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I71" s="6"/>
       <c r="J71" s="6"/>
       <c r="K71" s="6"/>
       <c r="L71" s="6"/>
       <c r="P71" s="6"/>
     </row>
-    <row r="72" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I72" s="6"/>
       <c r="J72" s="6"/>
       <c r="K72" s="6"/>
@@ -30781,7 +31263,7 @@
       <c r="P72" s="6"/>
       <c r="Q72" s="6"/>
     </row>
-    <row r="73" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I73" s="6"/>
       <c r="J73" s="6"/>
       <c r="K73" s="6"/>
@@ -30789,7 +31271,7 @@
       <c r="P73" s="6"/>
       <c r="Q73" s="6"/>
     </row>
-    <row r="74" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I74" s="6"/>
       <c r="J74" s="6"/>
       <c r="K74" s="6"/>
@@ -30797,27 +31279,27 @@
       <c r="P74" s="6"/>
       <c r="Q74" s="6"/>
     </row>
-    <row r="75" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:17" x14ac:dyDescent="0.3">
       <c r="P75" s="6"/>
       <c r="Q75" s="6"/>
     </row>
-    <row r="76" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:17" x14ac:dyDescent="0.3">
       <c r="P76" s="6"/>
       <c r="Q76" s="6"/>
     </row>
-    <row r="77" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:17" x14ac:dyDescent="0.3">
       <c r="P77" s="6"/>
       <c r="Q77" s="6"/>
     </row>
-    <row r="78" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:17" x14ac:dyDescent="0.3">
       <c r="P78" s="6"/>
       <c r="Q78" s="6"/>
     </row>
-    <row r="79" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:17" x14ac:dyDescent="0.3">
       <c r="P79" s="6"/>
       <c r="Q79" s="6"/>
     </row>
-    <row r="80" spans="9:17" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:17" x14ac:dyDescent="0.3">
       <c r="P80" s="6"/>
       <c r="Q80" s="6"/>
     </row>
@@ -30871,7 +31353,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -32787,8 +33269,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6748DF8D-1E96-42F5-BE18-DD686141E658}">
   <dimension ref="B2:M7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
added correlation matrices to SM variables and target
</commit_message>
<xml_diff>
--- a/New_DB.xlsx
+++ b/New_DB.xlsx
@@ -2,24 +2,25 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr hidePivotFieldList="1" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\MCC\Thesis\Project\2024_Project\new_election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5E88518-F7A6-4216-9FA1-FEEFB5DA0069}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AC85F-25B3-4C4C-8821-C068DAE75C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" activeTab="1" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
+    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" activeTab="2" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Galvez" sheetId="13" r:id="rId1"/>
     <sheet name="Claudia" sheetId="18" r:id="rId2"/>
     <sheet name="Maynez" sheetId="21" r:id="rId3"/>
-    <sheet name="Accounts" sheetId="6" r:id="rId4"/>
-    <sheet name="Polls" sheetId="20" r:id="rId5"/>
-    <sheet name="Vida Post" sheetId="22" r:id="rId6"/>
-    <sheet name="Results" sheetId="23" r:id="rId7"/>
+    <sheet name="Describe" sheetId="24" r:id="rId4"/>
+    <sheet name="Accounts" sheetId="6" r:id="rId5"/>
+    <sheet name="Polls" sheetId="20" r:id="rId6"/>
+    <sheet name="Vida Post" sheetId="22" r:id="rId7"/>
+    <sheet name="Results" sheetId="23" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -64,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="85">
   <si>
     <t>Candidate</t>
   </si>
@@ -310,6 +311,15 @@
   </si>
   <si>
     <t>MonthName</t>
+  </si>
+  <si>
+    <t>Xposts</t>
+  </si>
+  <si>
+    <t>Fbreacts</t>
+  </si>
+  <si>
+    <t>Total</t>
   </si>
 </sst>
 </file>
@@ -867,8 +877,8 @@
   <dimension ref="A1:XEU253"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P200" sqref="P200"/>
+      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="X13" sqref="X13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -11362,7 +11372,7 @@
         <v>20269</v>
       </c>
       <c r="R143" s="8">
-        <f t="shared" ref="R143:R192" si="59">Q143/P143</f>
+        <f t="shared" ref="R143:R194" si="59">Q143/P143</f>
         <v>6756.333333333333</v>
       </c>
       <c r="S143" s="6">
@@ -13913,7 +13923,7 @@
         <v>168393</v>
       </c>
       <c r="U178" s="8">
-        <f t="shared" ref="U178:U190" si="72">T178/S178</f>
+        <f t="shared" ref="U178:U194" si="72">T178/S178</f>
         <v>33678.6</v>
       </c>
     </row>
@@ -14250,15 +14260,15 @@
         <v>11059</v>
       </c>
       <c r="M183" s="6">
-        <f t="shared" ref="M183:M192" si="79">J183/I183</f>
+        <f t="shared" ref="M183:M194" si="79">J183/I183</f>
         <v>22150</v>
       </c>
       <c r="N183" s="6">
-        <f t="shared" ref="N183:N192" si="80">K183/I183</f>
+        <f t="shared" ref="N183:N194" si="80">K183/I183</f>
         <v>5078.625</v>
       </c>
       <c r="O183" s="8">
-        <f t="shared" ref="O183:O192" si="81">L183/I183</f>
+        <f t="shared" ref="O183:O194" si="81">L183/I183</f>
         <v>1382.375</v>
       </c>
       <c r="P183" s="6">
@@ -14810,15 +14820,15 @@
         <v>47600</v>
       </c>
       <c r="F191" s="6">
-        <f t="shared" ref="F191:F192" si="82">C191/B191</f>
+        <f t="shared" ref="F191:F194" si="82">C191/B191</f>
         <v>781.25</v>
       </c>
       <c r="G191" s="6">
-        <f t="shared" ref="G191:G192" si="83">D191/B191</f>
+        <f t="shared" ref="G191:G194" si="83">D191/B191</f>
         <v>2612.5</v>
       </c>
       <c r="H191" s="8">
-        <f t="shared" ref="H191:H192" si="84">E191/B191</f>
+        <f t="shared" ref="H191:H194" si="84">E191/B191</f>
         <v>5950</v>
       </c>
       <c r="I191" s="6">
@@ -14855,6 +14865,16 @@
         <f t="shared" si="59"/>
         <v>8362.4285714285706</v>
       </c>
+      <c r="S191" s="6">
+        <v>3</v>
+      </c>
+      <c r="T191" s="6">
+        <v>1512700</v>
+      </c>
+      <c r="U191" s="8">
+        <f t="shared" si="72"/>
+        <v>504233.33333333331</v>
+      </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A192" s="9">
@@ -14918,32 +14938,167 @@
         <f t="shared" si="59"/>
         <v>5408.1428571428569</v>
       </c>
-    </row>
-    <row r="193" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B193" s="6"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="6"/>
-      <c r="I193" s="6"/>
-      <c r="J193" s="6"/>
-      <c r="K193" s="6"/>
-      <c r="L193" s="6"/>
-      <c r="P193" s="6"/>
-      <c r="Q193" s="6"/>
-    </row>
-    <row r="194" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B194" s="6"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="6"/>
-      <c r="E194" s="6"/>
-      <c r="I194" s="6"/>
-      <c r="J194" s="6"/>
-      <c r="K194" s="6"/>
-      <c r="L194" s="6"/>
-      <c r="P194" s="6"/>
-      <c r="Q194" s="6"/>
-    </row>
-    <row r="195" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="S192" s="6">
+        <v>2</v>
+      </c>
+      <c r="T192" s="6">
+        <v>2570000</v>
+      </c>
+      <c r="U192" s="8">
+        <f t="shared" si="72"/>
+        <v>1285000</v>
+      </c>
+    </row>
+    <row r="193" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A193" s="9">
+        <v>45366</v>
+      </c>
+      <c r="B193" s="6">
+        <v>10</v>
+      </c>
+      <c r="C193" s="6">
+        <v>9082</v>
+      </c>
+      <c r="D193" s="6">
+        <v>29000</v>
+      </c>
+      <c r="E193" s="6">
+        <v>71000</v>
+      </c>
+      <c r="F193" s="6">
+        <f t="shared" si="82"/>
+        <v>908.2</v>
+      </c>
+      <c r="G193" s="6">
+        <f t="shared" si="83"/>
+        <v>2900</v>
+      </c>
+      <c r="H193" s="8">
+        <f t="shared" si="84"/>
+        <v>7100</v>
+      </c>
+      <c r="I193" s="6">
+        <v>10</v>
+      </c>
+      <c r="J193" s="6">
+        <v>265900</v>
+      </c>
+      <c r="K193" s="6">
+        <v>54348</v>
+      </c>
+      <c r="L193" s="6">
+        <v>10313</v>
+      </c>
+      <c r="M193" s="6">
+        <f t="shared" si="79"/>
+        <v>26590</v>
+      </c>
+      <c r="N193" s="6">
+        <f t="shared" si="80"/>
+        <v>5434.8</v>
+      </c>
+      <c r="O193" s="8">
+        <f t="shared" si="81"/>
+        <v>1031.3</v>
+      </c>
+      <c r="P193" s="6">
+        <v>7</v>
+      </c>
+      <c r="Q193" s="6">
+        <v>48775</v>
+      </c>
+      <c r="R193" s="8">
+        <f t="shared" si="59"/>
+        <v>6967.8571428571431</v>
+      </c>
+      <c r="S193" s="6">
+        <v>2</v>
+      </c>
+      <c r="T193" s="6">
+        <v>8200000</v>
+      </c>
+      <c r="U193" s="8">
+        <f t="shared" si="72"/>
+        <v>4100000</v>
+      </c>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A194" s="9">
+        <v>45367</v>
+      </c>
+      <c r="B194" s="6">
+        <v>9</v>
+      </c>
+      <c r="C194" s="6">
+        <v>9586</v>
+      </c>
+      <c r="D194" s="6">
+        <v>35400</v>
+      </c>
+      <c r="E194" s="6">
+        <v>86000</v>
+      </c>
+      <c r="F194" s="6">
+        <f t="shared" si="82"/>
+        <v>1065.1111111111111</v>
+      </c>
+      <c r="G194" s="6">
+        <f t="shared" si="83"/>
+        <v>3933.3333333333335</v>
+      </c>
+      <c r="H194" s="8">
+        <f t="shared" si="84"/>
+        <v>9555.5555555555547</v>
+      </c>
+      <c r="I194" s="6">
+        <v>9</v>
+      </c>
+      <c r="J194" s="6">
+        <v>117800</v>
+      </c>
+      <c r="K194" s="6">
+        <v>29659</v>
+      </c>
+      <c r="L194" s="6">
+        <v>10580</v>
+      </c>
+      <c r="M194" s="6">
+        <f t="shared" si="79"/>
+        <v>13088.888888888889</v>
+      </c>
+      <c r="N194" s="6">
+        <f t="shared" si="80"/>
+        <v>3295.4444444444443</v>
+      </c>
+      <c r="O194" s="8">
+        <f t="shared" si="81"/>
+        <v>1175.5555555555557</v>
+      </c>
+      <c r="P194" s="6">
+        <v>8</v>
+      </c>
+      <c r="Q194" s="6">
+        <v>66700</v>
+      </c>
+      <c r="R194" s="8">
+        <f t="shared" si="59"/>
+        <v>8337.5</v>
+      </c>
+      <c r="S194" s="6">
+        <v>2</v>
+      </c>
+      <c r="T194" s="6">
+        <v>26500</v>
+      </c>
+      <c r="U194" s="8">
+        <f t="shared" si="72"/>
+        <v>13250</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A195" s="9">
+        <v>45368</v>
+      </c>
       <c r="B195" s="6"/>
       <c r="C195" s="28"/>
       <c r="D195" s="6"/>
@@ -14955,7 +15110,10 @@
       <c r="P195" s="6"/>
       <c r="Q195" s="6"/>
     </row>
-    <row r="196" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A196" s="9">
+        <v>45369</v>
+      </c>
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
       <c r="D196" s="6"/>
@@ -14967,7 +15125,7 @@
       <c r="P196" s="6"/>
       <c r="Q196" s="6"/>
     </row>
-    <row r="197" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
       <c r="D197" s="6"/>
@@ -14979,7 +15137,7 @@
       <c r="P197" s="6"/>
       <c r="Q197" s="6"/>
     </row>
-    <row r="198" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="6"/>
@@ -14991,7 +15149,7 @@
       <c r="P198" s="6"/>
       <c r="Q198" s="6"/>
     </row>
-    <row r="199" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="6"/>
@@ -15003,7 +15161,8 @@
       <c r="P199" s="6"/>
       <c r="Q199" s="6"/>
     </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="6"/>
       <c r="E200" s="6"/>
@@ -15014,7 +15173,7 @@
       <c r="P200" s="6"/>
       <c r="Q200" s="6"/>
     </row>
-    <row r="201" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="6"/>
@@ -15026,7 +15185,7 @@
       <c r="P201" s="6"/>
       <c r="Q201" s="6"/>
     </row>
-    <row r="202" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="6"/>
@@ -15038,7 +15197,7 @@
       <c r="P202" s="6"/>
       <c r="Q202" s="6"/>
     </row>
-    <row r="203" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="6"/>
@@ -15050,8 +15209,7 @@
       <c r="P203" s="6"/>
       <c r="Q203" s="6"/>
     </row>
-    <row r="204" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B204" s="6"/>
+    <row r="204" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
       <c r="E204" s="6"/>
@@ -15062,7 +15220,7 @@
       <c r="P204" s="6"/>
       <c r="Q204" s="6"/>
     </row>
-    <row r="205" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="6"/>
@@ -15074,7 +15232,7 @@
       <c r="P205" s="6"/>
       <c r="Q205" s="6"/>
     </row>
-    <row r="206" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="6"/>
@@ -15086,7 +15244,7 @@
       <c r="P206" s="6"/>
       <c r="Q206" s="6"/>
     </row>
-    <row r="207" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="6"/>
@@ -15098,7 +15256,7 @@
       <c r="P207" s="6"/>
       <c r="Q207" s="6"/>
     </row>
-    <row r="208" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="6"/>
@@ -15187,6 +15345,7 @@
       <c r="C215" s="6"/>
       <c r="D215" s="6"/>
       <c r="E215" s="6"/>
+      <c r="I215" s="6"/>
       <c r="P215" s="6"/>
       <c r="Q215" s="6"/>
     </row>
@@ -15482,9 +15641,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC4418A-3538-4357-9158-8F79507C1D9F}">
   <dimension ref="A1:XET220"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A185" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="R198" sqref="R198"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -27312,15 +27471,15 @@
         <v>8422</v>
       </c>
       <c r="M162" s="6">
-        <f t="shared" ref="M162:M192" si="38">J162/I162</f>
+        <f t="shared" ref="M162:M194" si="38">J162/I162</f>
         <v>12650</v>
       </c>
       <c r="N162" s="6">
-        <f t="shared" ref="N162:N192" si="39">K162/I162</f>
+        <f t="shared" ref="N162:N194" si="39">K162/I162</f>
         <v>1410.8333333333333</v>
       </c>
       <c r="O162" s="8">
-        <f t="shared" ref="O162:O192" si="40">L162/I162</f>
+        <f t="shared" ref="O162:O194" si="40">L162/I162</f>
         <v>1403.6666666666667</v>
       </c>
       <c r="P162" s="6">
@@ -27693,7 +27852,7 @@
         <v>74697</v>
       </c>
       <c r="R167" s="8">
-        <f t="shared" ref="R167:R192" si="42">Q167/P167</f>
+        <f t="shared" ref="R167:R194" si="42">Q167/P167</f>
         <v>10671</v>
       </c>
       <c r="S167" s="6">
@@ -28576,7 +28735,7 @@
         <v>195200</v>
       </c>
       <c r="U179" s="8">
-        <f t="shared" ref="U179:U190" si="43">T179/S179</f>
+        <f t="shared" ref="U179:U194" si="43">T179/S179</f>
         <v>13942.857142857143</v>
       </c>
     </row>
@@ -29035,15 +29194,15 @@
         <v>39900</v>
       </c>
       <c r="F186" s="6">
-        <f t="shared" ref="F186:F192" si="44">C186/B186</f>
+        <f t="shared" ref="F186:F194" si="44">C186/B186</f>
         <v>802.5</v>
       </c>
       <c r="G186" s="6">
-        <f t="shared" ref="G186:G192" si="45">D186/B186</f>
+        <f t="shared" ref="G186:G194" si="45">D186/B186</f>
         <v>1642.9</v>
       </c>
       <c r="H186" s="8">
-        <f t="shared" ref="H186:H192" si="46">E186/B186</f>
+        <f t="shared" ref="H186:H194" si="46">E186/B186</f>
         <v>3990</v>
       </c>
       <c r="I186" s="6">
@@ -29445,6 +29604,16 @@
         <f t="shared" si="42"/>
         <v>7390.3846153846152</v>
       </c>
+      <c r="S191" s="6">
+        <v>4</v>
+      </c>
+      <c r="T191" s="6">
+        <v>407000</v>
+      </c>
+      <c r="U191" s="8">
+        <f t="shared" si="43"/>
+        <v>101750</v>
+      </c>
     </row>
     <row r="192" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A192" s="9">
@@ -29508,32 +29677,167 @@
         <f t="shared" si="42"/>
         <v>5045.4444444444443</v>
       </c>
-    </row>
-    <row r="193" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B193" s="6"/>
-      <c r="C193" s="6"/>
-      <c r="D193" s="6"/>
-      <c r="E193" s="6"/>
-      <c r="I193" s="6"/>
-      <c r="J193" s="6"/>
-      <c r="K193" s="6"/>
-      <c r="L193" s="6"/>
-      <c r="P193" s="6"/>
-      <c r="Q193" s="6"/>
-    </row>
-    <row r="194" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B194" s="6"/>
-      <c r="C194" s="6"/>
-      <c r="D194" s="6"/>
-      <c r="E194" s="6"/>
-      <c r="I194" s="6"/>
-      <c r="J194" s="6"/>
-      <c r="K194" s="6"/>
-      <c r="L194" s="6"/>
-      <c r="P194" s="6"/>
-      <c r="Q194" s="6"/>
-    </row>
-    <row r="195" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="S192" s="6">
+        <v>4</v>
+      </c>
+      <c r="T192" s="6">
+        <v>546800</v>
+      </c>
+      <c r="U192" s="8">
+        <f t="shared" si="43"/>
+        <v>136700</v>
+      </c>
+    </row>
+    <row r="193" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A193" s="9">
+        <v>45366</v>
+      </c>
+      <c r="B193" s="6">
+        <v>7</v>
+      </c>
+      <c r="C193" s="6">
+        <v>3947</v>
+      </c>
+      <c r="D193" s="6">
+        <v>10951</v>
+      </c>
+      <c r="E193" s="6">
+        <v>27200</v>
+      </c>
+      <c r="F193" s="6">
+        <f t="shared" si="44"/>
+        <v>563.85714285714289</v>
+      </c>
+      <c r="G193" s="6">
+        <f t="shared" si="45"/>
+        <v>1564.4285714285713</v>
+      </c>
+      <c r="H193" s="8">
+        <f t="shared" si="46"/>
+        <v>3885.7142857142858</v>
+      </c>
+      <c r="I193" s="6">
+        <v>13</v>
+      </c>
+      <c r="J193" s="6">
+        <v>245300</v>
+      </c>
+      <c r="K193" s="6">
+        <v>13692</v>
+      </c>
+      <c r="L193" s="6">
+        <v>16844</v>
+      </c>
+      <c r="M193" s="6">
+        <f t="shared" si="38"/>
+        <v>18869.23076923077</v>
+      </c>
+      <c r="N193" s="6">
+        <f t="shared" si="39"/>
+        <v>1053.2307692307693</v>
+      </c>
+      <c r="O193" s="8">
+        <f t="shared" si="40"/>
+        <v>1295.6923076923076</v>
+      </c>
+      <c r="P193" s="6">
+        <v>9</v>
+      </c>
+      <c r="Q193" s="6">
+        <v>43574</v>
+      </c>
+      <c r="R193" s="8">
+        <f t="shared" si="42"/>
+        <v>4841.5555555555557</v>
+      </c>
+      <c r="S193" s="6">
+        <v>3</v>
+      </c>
+      <c r="T193" s="6">
+        <v>111500</v>
+      </c>
+      <c r="U193" s="8">
+        <f t="shared" si="43"/>
+        <v>37166.666666666664</v>
+      </c>
+    </row>
+    <row r="194" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A194" s="9">
+        <v>45367</v>
+      </c>
+      <c r="B194" s="6">
+        <v>7</v>
+      </c>
+      <c r="C194" s="6">
+        <v>4506</v>
+      </c>
+      <c r="D194" s="6">
+        <v>12100</v>
+      </c>
+      <c r="E194" s="6">
+        <v>28400</v>
+      </c>
+      <c r="F194" s="6">
+        <f t="shared" si="44"/>
+        <v>643.71428571428567</v>
+      </c>
+      <c r="G194" s="6">
+        <f t="shared" si="45"/>
+        <v>1728.5714285714287</v>
+      </c>
+      <c r="H194" s="8">
+        <f t="shared" si="46"/>
+        <v>4057.1428571428573</v>
+      </c>
+      <c r="I194" s="6">
+        <v>9</v>
+      </c>
+      <c r="J194" s="6">
+        <v>78200</v>
+      </c>
+      <c r="K194" s="6">
+        <v>5355</v>
+      </c>
+      <c r="L194" s="6">
+        <v>9672</v>
+      </c>
+      <c r="M194" s="6">
+        <f t="shared" si="38"/>
+        <v>8688.8888888888887</v>
+      </c>
+      <c r="N194" s="6">
+        <f t="shared" si="39"/>
+        <v>595</v>
+      </c>
+      <c r="O194" s="8">
+        <f t="shared" si="40"/>
+        <v>1074.6666666666667</v>
+      </c>
+      <c r="P194" s="6">
+        <v>9</v>
+      </c>
+      <c r="Q194" s="6">
+        <v>29592</v>
+      </c>
+      <c r="R194" s="8">
+        <f t="shared" si="42"/>
+        <v>3288</v>
+      </c>
+      <c r="S194" s="6">
+        <v>5</v>
+      </c>
+      <c r="T194" s="6">
+        <v>246400</v>
+      </c>
+      <c r="U194" s="8">
+        <f t="shared" si="43"/>
+        <v>49280</v>
+      </c>
+    </row>
+    <row r="195" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A195" s="9">
+        <v>45368</v>
+      </c>
       <c r="B195" s="6"/>
       <c r="C195" s="6"/>
       <c r="D195" s="6"/>
@@ -29545,7 +29849,10 @@
       <c r="P195" s="6"/>
       <c r="Q195" s="6"/>
     </row>
-    <row r="196" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A196" s="9">
+        <v>45369</v>
+      </c>
       <c r="B196" s="6"/>
       <c r="C196" s="6"/>
       <c r="D196" s="6"/>
@@ -29557,7 +29864,7 @@
       <c r="P196" s="6"/>
       <c r="Q196" s="6"/>
     </row>
-    <row r="197" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B197" s="6"/>
       <c r="C197" s="6"/>
       <c r="D197" s="6"/>
@@ -29569,7 +29876,7 @@
       <c r="P197" s="6"/>
       <c r="Q197" s="6"/>
     </row>
-    <row r="198" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B198" s="6"/>
       <c r="C198" s="6"/>
       <c r="D198" s="6"/>
@@ -29581,7 +29888,7 @@
       <c r="P198" s="6"/>
       <c r="Q198" s="6"/>
     </row>
-    <row r="199" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B199" s="6"/>
       <c r="C199" s="6"/>
       <c r="D199" s="6"/>
@@ -29593,7 +29900,7 @@
       <c r="P199" s="6"/>
       <c r="Q199" s="6"/>
     </row>
-    <row r="200" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B200" s="6"/>
       <c r="C200" s="6"/>
       <c r="D200" s="6"/>
@@ -29605,7 +29912,7 @@
       <c r="P200" s="6"/>
       <c r="Q200" s="6"/>
     </row>
-    <row r="201" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B201" s="6"/>
       <c r="C201" s="6"/>
       <c r="D201" s="6"/>
@@ -29617,8 +29924,7 @@
       <c r="P201" s="6"/>
       <c r="Q201" s="6"/>
     </row>
-    <row r="202" spans="2:17" x14ac:dyDescent="0.3">
-      <c r="B202" s="6"/>
+    <row r="202" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C202" s="6"/>
       <c r="D202" s="6"/>
       <c r="E202" s="6"/>
@@ -29629,7 +29935,7 @@
       <c r="P202" s="6"/>
       <c r="Q202" s="6"/>
     </row>
-    <row r="203" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B203" s="6"/>
       <c r="C203" s="6"/>
       <c r="D203" s="6"/>
@@ -29641,7 +29947,7 @@
       <c r="P203" s="6"/>
       <c r="Q203" s="6"/>
     </row>
-    <row r="204" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
@@ -29653,7 +29959,7 @@
       <c r="P204" s="6"/>
       <c r="Q204" s="6"/>
     </row>
-    <row r="205" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B205" s="6"/>
       <c r="C205" s="6"/>
       <c r="D205" s="6"/>
@@ -29665,7 +29971,7 @@
       <c r="P205" s="6"/>
       <c r="Q205" s="6"/>
     </row>
-    <row r="206" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B206" s="6"/>
       <c r="C206" s="6"/>
       <c r="D206" s="6"/>
@@ -29677,7 +29983,7 @@
       <c r="P206" s="6"/>
       <c r="Q206" s="6"/>
     </row>
-    <row r="207" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B207" s="6"/>
       <c r="C207" s="6"/>
       <c r="D207" s="6"/>
@@ -29689,7 +29995,7 @@
       <c r="P207" s="6"/>
       <c r="Q207" s="6"/>
     </row>
-    <row r="208" spans="2:17" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B208" s="6"/>
       <c r="C208" s="6"/>
       <c r="D208" s="6"/>
@@ -29844,9 +30150,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8DF91097-4FB7-4052-890B-7AEB04A1F433}">
   <dimension ref="A1:V108"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A60" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J77" sqref="J77"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -31480,7 +31786,7 @@
         <v>8328</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" ref="R23:R66" si="9">Q23/P23</f>
+        <f t="shared" ref="R23:R68" si="9">Q23/P23</f>
         <v>1189.7142857142858</v>
       </c>
       <c r="S23" s="6">
@@ -33616,15 +33922,15 @@
         <v>1798</v>
       </c>
       <c r="M53" s="6">
-        <f t="shared" ref="M53:M66" si="20">J53/I53</f>
+        <f t="shared" ref="M53:M68" si="20">J53/I53</f>
         <v>5209.375</v>
       </c>
       <c r="N53" s="6">
-        <f t="shared" ref="N53:N66" si="21">K53/I53</f>
+        <f t="shared" ref="N53:N68" si="21">K53/I53</f>
         <v>1070.75</v>
       </c>
       <c r="O53" s="8">
-        <f t="shared" ref="O53:O66" si="22">L53/I53</f>
+        <f t="shared" ref="O53:O68" si="22">L53/I53</f>
         <v>224.75</v>
       </c>
       <c r="P53" s="6">
@@ -34320,15 +34626,15 @@
         <v>681</v>
       </c>
       <c r="F63" s="6">
-        <f t="shared" ref="F63:F66" si="27">C63/B63</f>
+        <f t="shared" ref="F63:F68" si="27">C63/B63</f>
         <v>40.142857142857146</v>
       </c>
       <c r="G63" s="6">
-        <f t="shared" ref="G63:G66" si="28">D63/B63</f>
+        <f t="shared" ref="G63:G68" si="28">D63/B63</f>
         <v>39.285714285714285</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" ref="H63:H66" si="29">E63/B63</f>
+        <f t="shared" ref="H63:H68" si="29">E63/B63</f>
         <v>97.285714285714292</v>
       </c>
       <c r="I63" s="6">
@@ -34372,7 +34678,7 @@
         <v>16721000</v>
       </c>
       <c r="U63" s="8">
-        <f t="shared" ref="U63:U64" si="30">T63/S63</f>
+        <f t="shared" ref="U63:U68" si="30">T63/S63</f>
         <v>1857888.888888889</v>
       </c>
     </row>
@@ -34449,7 +34755,7 @@
         <v>97000</v>
       </c>
     </row>
-    <row r="65" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A65" s="9">
         <v>45364</v>
       </c>
@@ -34511,8 +34817,18 @@
         <f t="shared" si="9"/>
         <v>688</v>
       </c>
-    </row>
-    <row r="66" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S65" s="6">
+        <v>1</v>
+      </c>
+      <c r="T65" s="6">
+        <v>237000</v>
+      </c>
+      <c r="U65" s="8">
+        <f t="shared" si="30"/>
+        <v>237000</v>
+      </c>
+    </row>
+    <row r="66" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A66" s="9">
         <v>45365</v>
       </c>
@@ -34574,32 +34890,167 @@
         <f t="shared" si="9"/>
         <v>1025</v>
       </c>
-    </row>
-    <row r="67" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B67" s="6"/>
-      <c r="C67" s="6"/>
-      <c r="D67" s="6"/>
-      <c r="E67" s="6"/>
-      <c r="I67" s="6"/>
-      <c r="J67" s="6"/>
-      <c r="K67" s="6"/>
-      <c r="L67" s="6"/>
-      <c r="P67" s="6"/>
-      <c r="Q67" s="6"/>
-    </row>
-    <row r="68" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B68" s="6"/>
-      <c r="C68" s="6"/>
-      <c r="D68" s="6"/>
-      <c r="E68" s="6"/>
-      <c r="I68" s="6"/>
-      <c r="J68" s="6"/>
-      <c r="K68" s="6"/>
-      <c r="L68" s="6"/>
-      <c r="P68" s="6"/>
-      <c r="Q68" s="6"/>
-    </row>
-    <row r="69" spans="1:18" x14ac:dyDescent="0.3">
+      <c r="S66" s="6">
+        <v>5</v>
+      </c>
+      <c r="T66" s="6">
+        <v>1267000</v>
+      </c>
+      <c r="U66" s="8">
+        <f t="shared" si="30"/>
+        <v>253400</v>
+      </c>
+    </row>
+    <row r="67" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A67" s="9">
+        <v>45366</v>
+      </c>
+      <c r="B67" s="6">
+        <v>5</v>
+      </c>
+      <c r="C67" s="6">
+        <v>303</v>
+      </c>
+      <c r="D67" s="6">
+        <v>207</v>
+      </c>
+      <c r="E67" s="6">
+        <v>458</v>
+      </c>
+      <c r="F67" s="6">
+        <f t="shared" si="27"/>
+        <v>60.6</v>
+      </c>
+      <c r="G67" s="6">
+        <f t="shared" si="28"/>
+        <v>41.4</v>
+      </c>
+      <c r="H67" s="8">
+        <f t="shared" si="29"/>
+        <v>91.6</v>
+      </c>
+      <c r="I67" s="6">
+        <v>9</v>
+      </c>
+      <c r="J67" s="6">
+        <v>15567</v>
+      </c>
+      <c r="K67" s="6">
+        <v>3946</v>
+      </c>
+      <c r="L67" s="6">
+        <v>1162</v>
+      </c>
+      <c r="M67" s="6">
+        <f t="shared" si="20"/>
+        <v>1729.6666666666667</v>
+      </c>
+      <c r="N67" s="6">
+        <f t="shared" si="21"/>
+        <v>438.44444444444446</v>
+      </c>
+      <c r="O67" s="8">
+        <f t="shared" si="22"/>
+        <v>129.11111111111111</v>
+      </c>
+      <c r="P67" s="6">
+        <v>7</v>
+      </c>
+      <c r="Q67" s="6">
+        <v>5949</v>
+      </c>
+      <c r="R67" s="8">
+        <f t="shared" si="9"/>
+        <v>849.85714285714289</v>
+      </c>
+      <c r="S67" s="6">
+        <v>2</v>
+      </c>
+      <c r="T67" s="6">
+        <v>819000</v>
+      </c>
+      <c r="U67" s="8">
+        <f t="shared" si="30"/>
+        <v>409500</v>
+      </c>
+    </row>
+    <row r="68" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A68" s="9">
+        <v>45367</v>
+      </c>
+      <c r="B68" s="6">
+        <v>5</v>
+      </c>
+      <c r="C68" s="6">
+        <v>227</v>
+      </c>
+      <c r="D68" s="6">
+        <v>191</v>
+      </c>
+      <c r="E68" s="6">
+        <v>436</v>
+      </c>
+      <c r="F68" s="6">
+        <f t="shared" si="27"/>
+        <v>45.4</v>
+      </c>
+      <c r="G68" s="6">
+        <f t="shared" si="28"/>
+        <v>38.200000000000003</v>
+      </c>
+      <c r="H68" s="8">
+        <f t="shared" si="29"/>
+        <v>87.2</v>
+      </c>
+      <c r="I68" s="6">
+        <v>7</v>
+      </c>
+      <c r="J68" s="6">
+        <v>9573</v>
+      </c>
+      <c r="K68" s="6">
+        <v>2335</v>
+      </c>
+      <c r="L68" s="6">
+        <v>1152</v>
+      </c>
+      <c r="M68" s="6">
+        <f t="shared" si="20"/>
+        <v>1367.5714285714287</v>
+      </c>
+      <c r="N68" s="6">
+        <f t="shared" si="21"/>
+        <v>333.57142857142856</v>
+      </c>
+      <c r="O68" s="8">
+        <f t="shared" si="22"/>
+        <v>164.57142857142858</v>
+      </c>
+      <c r="P68" s="6">
+        <v>7</v>
+      </c>
+      <c r="Q68" s="6">
+        <v>4955</v>
+      </c>
+      <c r="R68" s="8">
+        <f t="shared" si="9"/>
+        <v>707.85714285714289</v>
+      </c>
+      <c r="S68" s="6">
+        <v>8</v>
+      </c>
+      <c r="T68" s="6">
+        <v>4521000</v>
+      </c>
+      <c r="U68" s="8">
+        <f t="shared" si="30"/>
+        <v>565125</v>
+      </c>
+    </row>
+    <row r="69" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A69" s="9">
+        <v>45368</v>
+      </c>
       <c r="B69" s="6"/>
       <c r="C69" s="6"/>
       <c r="D69" s="6"/>
@@ -34611,7 +35062,10 @@
       <c r="P69" s="6"/>
       <c r="Q69" s="6"/>
     </row>
-    <row r="70" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A70" s="9">
+        <v>45369</v>
+      </c>
       <c r="B70" s="6"/>
       <c r="C70" s="6"/>
       <c r="D70" s="6"/>
@@ -34623,7 +35077,7 @@
       <c r="P70" s="6"/>
       <c r="Q70" s="6"/>
     </row>
-    <row r="71" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B71" s="6"/>
       <c r="C71" s="6"/>
       <c r="D71" s="6"/>
@@ -34635,7 +35089,7 @@
       <c r="P71" s="6"/>
       <c r="Q71" s="6"/>
     </row>
-    <row r="72" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B72" s="6"/>
       <c r="C72" s="6"/>
       <c r="D72" s="6"/>
@@ -34647,7 +35101,7 @@
       <c r="P72" s="6"/>
       <c r="Q72" s="6"/>
     </row>
-    <row r="73" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B73" s="6"/>
       <c r="C73" s="6"/>
       <c r="D73" s="6"/>
@@ -34659,8 +35113,7 @@
       <c r="P73" s="6"/>
       <c r="Q73" s="6"/>
     </row>
-    <row r="74" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="B74" s="6"/>
+    <row r="74" spans="1:21" x14ac:dyDescent="0.3">
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -34671,17 +35124,19 @@
       <c r="P74" s="6"/>
       <c r="Q74" s="6"/>
     </row>
-    <row r="75" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B75" s="6"/>
       <c r="C75" s="6"/>
       <c r="D75" s="6"/>
       <c r="E75" s="6"/>
+      <c r="I75" s="6"/>
       <c r="J75" s="6"/>
       <c r="K75" s="6"/>
       <c r="L75" s="6"/>
       <c r="P75" s="6"/>
       <c r="Q75" s="6"/>
     </row>
-    <row r="76" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B76" s="6"/>
       <c r="C76" s="6"/>
       <c r="D76" s="6"/>
@@ -34693,7 +35148,7 @@
       <c r="P76" s="6"/>
       <c r="Q76" s="6"/>
     </row>
-    <row r="77" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B77" s="6"/>
       <c r="C77" s="6"/>
       <c r="D77" s="6"/>
@@ -34705,7 +35160,7 @@
       <c r="P77" s="6"/>
       <c r="Q77" s="6"/>
     </row>
-    <row r="78" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B78" s="6"/>
       <c r="C78" s="6"/>
       <c r="D78" s="6"/>
@@ -34717,7 +35172,7 @@
       <c r="P78" s="6"/>
       <c r="Q78" s="6"/>
     </row>
-    <row r="79" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B79" s="6"/>
       <c r="C79" s="6"/>
       <c r="D79" s="6"/>
@@ -34729,7 +35184,7 @@
       <c r="P79" s="6"/>
       <c r="Q79" s="6"/>
     </row>
-    <row r="80" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B80" s="6"/>
       <c r="C80" s="6"/>
       <c r="D80" s="6"/>
@@ -34968,6 +35423,485 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346A044C-6F3E-436F-84AC-DB98BA731517}">
+  <dimension ref="A2:M22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>919</v>
+      </c>
+      <c r="C3">
+        <v>681403</v>
+      </c>
+      <c r="D3">
+        <v>1230276</v>
+      </c>
+      <c r="E3">
+        <v>3481884</v>
+      </c>
+      <c r="F3">
+        <v>1248</v>
+      </c>
+      <c r="G3">
+        <v>7505763</v>
+      </c>
+      <c r="H3">
+        <v>931280</v>
+      </c>
+      <c r="I3">
+        <v>707847</v>
+      </c>
+      <c r="J3">
+        <v>923</v>
+      </c>
+      <c r="K3">
+        <v>4848438</v>
+      </c>
+      <c r="L3">
+        <v>349</v>
+      </c>
+      <c r="M3">
+        <v>10688244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <v>510</v>
+      </c>
+      <c r="D4">
+        <v>1500</v>
+      </c>
+      <c r="E4">
+        <v>4100</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>9500</v>
+      </c>
+      <c r="I4">
+        <v>1279</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <v>13151</v>
+      </c>
+      <c r="D5">
+        <v>25456</v>
+      </c>
+      <c r="E5">
+        <v>81468</v>
+      </c>
+      <c r="G5">
+        <v>187100</v>
+      </c>
+      <c r="H5">
+        <v>24800</v>
+      </c>
+      <c r="I5">
+        <v>25926</v>
+      </c>
+      <c r="K5">
+        <v>161665</v>
+      </c>
+      <c r="M5">
+        <v>847671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>4635.3945578231296</v>
+      </c>
+      <c r="D6">
+        <v>8369.224489795919</v>
+      </c>
+      <c r="E6">
+        <v>23686.285714285714</v>
+      </c>
+      <c r="G6">
+        <v>51059.612244897959</v>
+      </c>
+      <c r="H6">
+        <v>6335.2380952380954</v>
+      </c>
+      <c r="I6">
+        <v>4815.2857142857147</v>
+      </c>
+      <c r="K6">
+        <v>32982.571428571428</v>
+      </c>
+      <c r="M6">
+        <v>72709.142857142855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>3917</v>
+      </c>
+      <c r="D7">
+        <v>7700</v>
+      </c>
+      <c r="E7">
+        <v>22100</v>
+      </c>
+      <c r="G7">
+        <v>38400</v>
+      </c>
+      <c r="H7">
+        <v>5474</v>
+      </c>
+      <c r="I7">
+        <v>4422</v>
+      </c>
+      <c r="K7">
+        <v>28016</v>
+      </c>
+      <c r="M7">
+        <v>18395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>2623.895375038468</v>
+      </c>
+      <c r="D8">
+        <v>3842.9305202547876</v>
+      </c>
+      <c r="E8">
+        <v>11596.721585614037</v>
+      </c>
+      <c r="G8">
+        <v>37255.368355915067</v>
+      </c>
+      <c r="H8">
+        <v>4025.0868370337184</v>
+      </c>
+      <c r="I8">
+        <v>2682.5965238158797</v>
+      </c>
+      <c r="K8">
+        <v>22670.2202970123</v>
+      </c>
+      <c r="M8">
+        <v>131648.55887015644</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>681403</v>
+      </c>
+      <c r="C12">
+        <v>510</v>
+      </c>
+      <c r="D12">
+        <v>13151</v>
+      </c>
+      <c r="E12">
+        <v>4635.3945578231296</v>
+      </c>
+      <c r="F12">
+        <v>3917</v>
+      </c>
+      <c r="G12">
+        <v>2623.895375038468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1230276</v>
+      </c>
+      <c r="C13">
+        <v>1500</v>
+      </c>
+      <c r="D13">
+        <v>25456</v>
+      </c>
+      <c r="E13">
+        <v>8369.224489795919</v>
+      </c>
+      <c r="F13">
+        <v>7700</v>
+      </c>
+      <c r="G13">
+        <v>3842.9305202547876</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>3481884</v>
+      </c>
+      <c r="C14">
+        <v>4100</v>
+      </c>
+      <c r="D14">
+        <v>81468</v>
+      </c>
+      <c r="E14">
+        <v>23686.285714285714</v>
+      </c>
+      <c r="F14">
+        <v>22100</v>
+      </c>
+      <c r="G14">
+        <v>11596.721585614037</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16">
+        <v>7505763</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>187100</v>
+      </c>
+      <c r="E16">
+        <v>51059.612244897959</v>
+      </c>
+      <c r="F16">
+        <v>38400</v>
+      </c>
+      <c r="G16">
+        <v>37255.368355915067</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>931280</v>
+      </c>
+      <c r="C17">
+        <v>9500</v>
+      </c>
+      <c r="D17">
+        <v>24800</v>
+      </c>
+      <c r="E17">
+        <v>6335.2380952380954</v>
+      </c>
+      <c r="F17">
+        <v>5474</v>
+      </c>
+      <c r="G17">
+        <v>4025.0868370337184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>707847</v>
+      </c>
+      <c r="C18">
+        <v>1279</v>
+      </c>
+      <c r="D18">
+        <v>25926</v>
+      </c>
+      <c r="E18">
+        <v>4815.2857142857147</v>
+      </c>
+      <c r="F18">
+        <v>4422</v>
+      </c>
+      <c r="G18">
+        <v>2682.5965238158797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>4848438</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>161665</v>
+      </c>
+      <c r="E20">
+        <v>32982.571428571428</v>
+      </c>
+      <c r="F20">
+        <v>28016</v>
+      </c>
+      <c r="G20">
+        <v>22670.2202970123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>10688244</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>847671</v>
+      </c>
+      <c r="E22">
+        <v>72709.142857142855</v>
+      </c>
+      <c r="F22">
+        <v>18395</v>
+      </c>
+      <c r="G22">
+        <v>131648.55887015644</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AAE58A-8A5A-4C93-AE14-DE5004288388}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -35026,7 +35960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62C3539-067A-49FB-A3DE-0B279692F912}">
   <dimension ref="A1:T42"/>
   <sheetViews>
@@ -36695,7 +37629,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC47CE33-EEC3-446C-940D-05592E4B50CB}">
   <dimension ref="A1:N8"/>
   <sheetViews>
@@ -37007,7 +37941,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6748DF8D-1E96-42F5-BE18-DD686141E658}">
   <dimension ref="B2:M9"/>
   <sheetViews>

</xml_diff>

<commit_message>
corr matrix new side
</commit_message>
<xml_diff>
--- a/New_DB.xlsx
+++ b/New_DB.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\usuario\Documents\MCC\Thesis\Project\2024_Project\new_election\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{281AC85F-25B3-4C4C-8821-C068DAE75C00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B983CA6F-D5CA-46BD-81AB-EE30E709010A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-118" yWindow="-118" windowWidth="25370" windowHeight="13759" tabRatio="819" activeTab="2" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
+    <workbookView xWindow="12567" yWindow="0" windowWidth="12568" windowHeight="13523" tabRatio="819" activeTab="2" xr2:uid="{13AFDAF7-A95F-4D3C-B348-D29B9628D89F}"/>
   </bookViews>
   <sheets>
     <sheet name="Galvez" sheetId="13" r:id="rId1"/>
     <sheet name="Claudia" sheetId="18" r:id="rId2"/>
     <sheet name="Maynez" sheetId="21" r:id="rId3"/>
-    <sheet name="Describe" sheetId="24" r:id="rId4"/>
-    <sheet name="Accounts" sheetId="6" r:id="rId5"/>
-    <sheet name="Polls" sheetId="20" r:id="rId6"/>
-    <sheet name="Vida Post" sheetId="22" r:id="rId7"/>
-    <sheet name="Results" sheetId="23" r:id="rId8"/>
+    <sheet name="Accounts" sheetId="6" r:id="rId4"/>
+    <sheet name="Polls" sheetId="20" r:id="rId5"/>
+    <sheet name="Vida Post" sheetId="22" r:id="rId6"/>
+    <sheet name="Results" sheetId="23" r:id="rId7"/>
+    <sheet name="Describe" sheetId="24" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -474,7 +474,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -537,9 +537,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -878,7 +875,7 @@
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="X13" sqref="X13"/>
+      <selection pane="bottomLeft" activeCell="A200" sqref="A200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -904,34 +901,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21 16252:16375" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="29" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="29" t="s">
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="31"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
     </row>
     <row r="2" spans="1:21 16252:16375" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -11372,7 +11369,7 @@
         <v>20269</v>
       </c>
       <c r="R143" s="8">
-        <f t="shared" ref="R143:R194" si="59">Q143/P143</f>
+        <f t="shared" ref="R143:R196" si="59">Q143/P143</f>
         <v>6756.333333333333</v>
       </c>
       <c r="S143" s="6">
@@ -14260,15 +14257,15 @@
         <v>11059</v>
       </c>
       <c r="M183" s="6">
-        <f t="shared" ref="M183:M194" si="79">J183/I183</f>
+        <f t="shared" ref="M183:M196" si="79">J183/I183</f>
         <v>22150</v>
       </c>
       <c r="N183" s="6">
-        <f t="shared" ref="N183:N194" si="80">K183/I183</f>
+        <f t="shared" ref="N183:N196" si="80">K183/I183</f>
         <v>5078.625</v>
       </c>
       <c r="O183" s="8">
-        <f t="shared" ref="O183:O194" si="81">L183/I183</f>
+        <f t="shared" ref="O183:O196" si="81">L183/I183</f>
         <v>1382.375</v>
       </c>
       <c r="P183" s="6">
@@ -14820,15 +14817,15 @@
         <v>47600</v>
       </c>
       <c r="F191" s="6">
-        <f t="shared" ref="F191:F194" si="82">C191/B191</f>
+        <f t="shared" ref="F191:F196" si="82">C191/B191</f>
         <v>781.25</v>
       </c>
       <c r="G191" s="6">
-        <f t="shared" ref="G191:G194" si="83">D191/B191</f>
+        <f t="shared" ref="G191:G196" si="83">D191/B191</f>
         <v>2612.5</v>
       </c>
       <c r="H191" s="8">
-        <f t="shared" ref="H191:H194" si="84">E191/B191</f>
+        <f t="shared" ref="H191:H196" si="84">E191/B191</f>
         <v>5950</v>
       </c>
       <c r="I191" s="6">
@@ -15099,31 +15096,127 @@
       <c r="A195" s="9">
         <v>45368</v>
       </c>
-      <c r="B195" s="6"/>
-      <c r="C195" s="28"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="28"/>
-      <c r="I195" s="6"/>
-      <c r="J195" s="6"/>
-      <c r="K195" s="6"/>
-      <c r="L195" s="6"/>
-      <c r="P195" s="6"/>
-      <c r="Q195" s="6"/>
+      <c r="B195" s="6">
+        <v>9</v>
+      </c>
+      <c r="C195" s="6">
+        <v>7655</v>
+      </c>
+      <c r="D195" s="6">
+        <v>27700</v>
+      </c>
+      <c r="E195" s="6">
+        <v>75700</v>
+      </c>
+      <c r="F195" s="6">
+        <f t="shared" si="82"/>
+        <v>850.55555555555554</v>
+      </c>
+      <c r="G195" s="6">
+        <f t="shared" si="83"/>
+        <v>3077.7777777777778</v>
+      </c>
+      <c r="H195" s="8">
+        <f t="shared" si="84"/>
+        <v>8411.1111111111113</v>
+      </c>
+      <c r="I195" s="6">
+        <v>10</v>
+      </c>
+      <c r="J195" s="6">
+        <v>256200</v>
+      </c>
+      <c r="K195" s="6">
+        <v>81986</v>
+      </c>
+      <c r="L195" s="6">
+        <v>14503</v>
+      </c>
+      <c r="M195" s="6">
+        <f t="shared" si="79"/>
+        <v>25620</v>
+      </c>
+      <c r="N195" s="6">
+        <f t="shared" si="80"/>
+        <v>8198.6</v>
+      </c>
+      <c r="O195" s="8">
+        <f t="shared" si="81"/>
+        <v>1450.3</v>
+      </c>
+      <c r="P195" s="6">
+        <v>8</v>
+      </c>
+      <c r="Q195" s="6">
+        <v>113729</v>
+      </c>
+      <c r="R195" s="8">
+        <f t="shared" si="59"/>
+        <v>14216.125</v>
+      </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A196" s="9">
         <v>45369</v>
       </c>
-      <c r="B196" s="6"/>
-      <c r="C196" s="6"/>
-      <c r="D196" s="6"/>
-      <c r="E196" s="6"/>
-      <c r="I196" s="6"/>
-      <c r="J196" s="6"/>
-      <c r="K196" s="6"/>
-      <c r="L196" s="6"/>
-      <c r="P196" s="6"/>
-      <c r="Q196" s="6"/>
+      <c r="B196" s="6">
+        <v>13</v>
+      </c>
+      <c r="C196" s="6">
+        <v>11618</v>
+      </c>
+      <c r="D196" s="6">
+        <v>37758</v>
+      </c>
+      <c r="E196" s="6">
+        <v>90600</v>
+      </c>
+      <c r="F196" s="6">
+        <f t="shared" si="82"/>
+        <v>893.69230769230774</v>
+      </c>
+      <c r="G196" s="6">
+        <f t="shared" si="83"/>
+        <v>2904.4615384615386</v>
+      </c>
+      <c r="H196" s="8">
+        <f t="shared" si="84"/>
+        <v>6969.2307692307695</v>
+      </c>
+      <c r="I196" s="6">
+        <v>12</v>
+      </c>
+      <c r="J196" s="6">
+        <v>343200</v>
+      </c>
+      <c r="K196" s="6">
+        <v>76724</v>
+      </c>
+      <c r="L196" s="6">
+        <v>16974</v>
+      </c>
+      <c r="M196" s="6">
+        <f t="shared" si="79"/>
+        <v>28600</v>
+      </c>
+      <c r="N196" s="6">
+        <f t="shared" si="80"/>
+        <v>6393.666666666667</v>
+      </c>
+      <c r="O196" s="8">
+        <f t="shared" si="81"/>
+        <v>1414.5</v>
+      </c>
+      <c r="P196" s="6">
+        <v>7</v>
+      </c>
+      <c r="Q196" s="6">
+        <v>41233</v>
+      </c>
+      <c r="R196" s="8">
+        <f t="shared" si="59"/>
+        <v>5890.4285714285716</v>
+      </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B197" s="6"/>
@@ -15210,6 +15303,7 @@
       <c r="Q203" s="6"/>
     </row>
     <row r="204" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B204" s="6"/>
       <c r="C204" s="6"/>
       <c r="D204" s="6"/>
       <c r="E204" s="6"/>
@@ -15346,6 +15440,9 @@
       <c r="D215" s="6"/>
       <c r="E215" s="6"/>
       <c r="I215" s="6"/>
+      <c r="J215" s="6"/>
+      <c r="K215" s="6"/>
+      <c r="L215" s="6"/>
       <c r="P215" s="6"/>
       <c r="Q215" s="6"/>
     </row>
@@ -15354,6 +15451,10 @@
       <c r="C216" s="6"/>
       <c r="D216" s="6"/>
       <c r="E216" s="6"/>
+      <c r="I216" s="6"/>
+      <c r="J216" s="6"/>
+      <c r="K216" s="6"/>
+      <c r="L216" s="6"/>
       <c r="P216" s="6"/>
       <c r="Q216" s="6"/>
     </row>
@@ -15362,6 +15463,10 @@
       <c r="C217" s="6"/>
       <c r="D217" s="6"/>
       <c r="E217" s="6"/>
+      <c r="I217" s="6"/>
+      <c r="J217" s="6"/>
+      <c r="K217" s="6"/>
+      <c r="L217" s="6"/>
       <c r="P217" s="6"/>
       <c r="Q217" s="6"/>
     </row>
@@ -15370,6 +15475,10 @@
       <c r="C218" s="6"/>
       <c r="D218" s="6"/>
       <c r="E218" s="6"/>
+      <c r="I218" s="6"/>
+      <c r="J218" s="6"/>
+      <c r="K218" s="6"/>
+      <c r="L218" s="6"/>
       <c r="P218" s="6"/>
       <c r="Q218" s="6"/>
     </row>
@@ -15378,6 +15487,10 @@
       <c r="C219" s="6"/>
       <c r="D219" s="6"/>
       <c r="E219" s="6"/>
+      <c r="I219" s="6"/>
+      <c r="J219" s="6"/>
+      <c r="K219" s="6"/>
+      <c r="L219" s="6"/>
       <c r="P219" s="6"/>
       <c r="Q219" s="6"/>
     </row>
@@ -15386,6 +15499,7 @@
       <c r="C220" s="6"/>
       <c r="D220" s="6"/>
       <c r="E220" s="6"/>
+      <c r="I220" s="6"/>
       <c r="P220" s="6"/>
     </row>
     <row r="221" spans="2:17" x14ac:dyDescent="0.3">
@@ -15639,11 +15753,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2BC4418A-3538-4357-9158-8F79507C1D9F}">
-  <dimension ref="A1:XET220"/>
+  <dimension ref="A1:XET225"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A190" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D18" sqref="D18"/>
+    <sheetView topLeftCell="M1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A191" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="T208" sqref="T208"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -15666,34 +15780,34 @@
   <sheetData>
     <row r="1" spans="1:21 16251:16374" x14ac:dyDescent="0.3">
       <c r="A1" s="7"/>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="29" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="29" t="s">
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="31"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
     </row>
     <row r="2" spans="1:21 16251:16374" s="10" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="8" t="s">
@@ -27471,15 +27585,15 @@
         <v>8422</v>
       </c>
       <c r="M162" s="6">
-        <f t="shared" ref="M162:M194" si="38">J162/I162</f>
+        <f t="shared" ref="M162:M196" si="38">J162/I162</f>
         <v>12650</v>
       </c>
       <c r="N162" s="6">
-        <f t="shared" ref="N162:N194" si="39">K162/I162</f>
+        <f t="shared" ref="N162:N196" si="39">K162/I162</f>
         <v>1410.8333333333333</v>
       </c>
       <c r="O162" s="8">
-        <f t="shared" ref="O162:O194" si="40">L162/I162</f>
+        <f t="shared" ref="O162:O196" si="40">L162/I162</f>
         <v>1403.6666666666667</v>
       </c>
       <c r="P162" s="6">
@@ -27852,7 +27966,7 @@
         <v>74697</v>
       </c>
       <c r="R167" s="8">
-        <f t="shared" ref="R167:R194" si="42">Q167/P167</f>
+        <f t="shared" ref="R167:R196" si="42">Q167/P167</f>
         <v>10671</v>
       </c>
       <c r="S167" s="6">
@@ -29194,15 +29308,15 @@
         <v>39900</v>
       </c>
       <c r="F186" s="6">
-        <f t="shared" ref="F186:F194" si="44">C186/B186</f>
+        <f t="shared" ref="F186:F196" si="44">C186/B186</f>
         <v>802.5</v>
       </c>
       <c r="G186" s="6">
-        <f t="shared" ref="G186:G194" si="45">D186/B186</f>
+        <f t="shared" ref="G186:G196" si="45">D186/B186</f>
         <v>1642.9</v>
       </c>
       <c r="H186" s="8">
-        <f t="shared" ref="H186:H194" si="46">E186/B186</f>
+        <f t="shared" ref="H186:H196" si="46">E186/B186</f>
         <v>3990</v>
       </c>
       <c r="I186" s="6">
@@ -29838,31 +29952,127 @@
       <c r="A195" s="9">
         <v>45368</v>
       </c>
-      <c r="B195" s="6"/>
-      <c r="C195" s="6"/>
-      <c r="D195" s="6"/>
-      <c r="E195" s="6"/>
-      <c r="I195" s="6"/>
-      <c r="J195" s="6"/>
-      <c r="K195" s="6"/>
-      <c r="L195" s="6"/>
-      <c r="P195" s="6"/>
-      <c r="Q195" s="6"/>
+      <c r="B195" s="6">
+        <v>8</v>
+      </c>
+      <c r="C195" s="6">
+        <v>7075</v>
+      </c>
+      <c r="D195" s="6">
+        <v>16100</v>
+      </c>
+      <c r="E195" s="6">
+        <v>43900</v>
+      </c>
+      <c r="F195" s="6">
+        <f t="shared" si="44"/>
+        <v>884.375</v>
+      </c>
+      <c r="G195" s="6">
+        <f t="shared" si="45"/>
+        <v>2012.5</v>
+      </c>
+      <c r="H195" s="8">
+        <f t="shared" si="46"/>
+        <v>5487.5</v>
+      </c>
+      <c r="I195" s="6">
+        <v>7</v>
+      </c>
+      <c r="J195" s="6">
+        <v>152000</v>
+      </c>
+      <c r="K195" s="6">
+        <v>10232</v>
+      </c>
+      <c r="L195" s="6">
+        <v>12499</v>
+      </c>
+      <c r="M195" s="6">
+        <f t="shared" si="38"/>
+        <v>21714.285714285714</v>
+      </c>
+      <c r="N195" s="6">
+        <f t="shared" si="39"/>
+        <v>1461.7142857142858</v>
+      </c>
+      <c r="O195" s="8">
+        <f t="shared" si="40"/>
+        <v>1785.5714285714287</v>
+      </c>
+      <c r="P195" s="6">
+        <v>18</v>
+      </c>
+      <c r="Q195" s="6">
+        <v>111801</v>
+      </c>
+      <c r="R195" s="8">
+        <f t="shared" si="42"/>
+        <v>6211.166666666667</v>
+      </c>
     </row>
     <row r="196" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A196" s="9">
         <v>45369</v>
       </c>
-      <c r="B196" s="6"/>
-      <c r="C196" s="6"/>
-      <c r="D196" s="6"/>
-      <c r="E196" s="6"/>
-      <c r="I196" s="6"/>
-      <c r="J196" s="6"/>
-      <c r="K196" s="6"/>
-      <c r="L196" s="6"/>
-      <c r="P196" s="6"/>
-      <c r="Q196" s="6"/>
+      <c r="B196" s="6">
+        <v>8</v>
+      </c>
+      <c r="C196" s="6">
+        <v>4469</v>
+      </c>
+      <c r="D196" s="6">
+        <v>11434</v>
+      </c>
+      <c r="E196" s="6">
+        <v>29700</v>
+      </c>
+      <c r="F196" s="6">
+        <f t="shared" si="44"/>
+        <v>558.625</v>
+      </c>
+      <c r="G196" s="6">
+        <f t="shared" si="45"/>
+        <v>1429.25</v>
+      </c>
+      <c r="H196" s="8">
+        <f t="shared" si="46"/>
+        <v>3712.5</v>
+      </c>
+      <c r="I196" s="6">
+        <v>11</v>
+      </c>
+      <c r="J196" s="6">
+        <v>79000</v>
+      </c>
+      <c r="K196" s="6">
+        <v>6379</v>
+      </c>
+      <c r="L196" s="6">
+        <v>8512</v>
+      </c>
+      <c r="M196" s="6">
+        <f t="shared" si="38"/>
+        <v>7181.818181818182</v>
+      </c>
+      <c r="N196" s="6">
+        <f t="shared" si="39"/>
+        <v>579.90909090909088</v>
+      </c>
+      <c r="O196" s="8">
+        <f t="shared" si="40"/>
+        <v>773.81818181818187</v>
+      </c>
+      <c r="P196" s="6">
+        <v>9</v>
+      </c>
+      <c r="Q196" s="6">
+        <v>51182</v>
+      </c>
+      <c r="R196" s="8">
+        <f t="shared" si="42"/>
+        <v>5686.8888888888887</v>
+      </c>
     </row>
     <row r="197" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B197" s="6"/>
@@ -29925,6 +30135,7 @@
       <c r="Q201" s="6"/>
     </row>
     <row r="202" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B202" s="6"/>
       <c r="C202" s="6"/>
       <c r="D202" s="6"/>
       <c r="E202" s="6"/>
@@ -30101,6 +30312,7 @@
       <c r="K216" s="6"/>
       <c r="L216" s="6"/>
       <c r="P216" s="6"/>
+      <c r="Q216" s="6"/>
     </row>
     <row r="217" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B217" s="6"/>
@@ -30111,6 +30323,8 @@
       <c r="J217" s="6"/>
       <c r="K217" s="6"/>
       <c r="L217" s="6"/>
+      <c r="P217" s="6"/>
+      <c r="Q217" s="6"/>
     </row>
     <row r="218" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B218" s="6"/>
@@ -30121,6 +30335,8 @@
       <c r="J218" s="6"/>
       <c r="K218" s="6"/>
       <c r="L218" s="6"/>
+      <c r="P218" s="6"/>
+      <c r="Q218" s="6"/>
     </row>
     <row r="219" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B219" s="6"/>
@@ -30131,9 +30347,32 @@
       <c r="J219" s="6"/>
       <c r="K219" s="6"/>
       <c r="L219" s="6"/>
+      <c r="P219" s="6"/>
+      <c r="Q219" s="6"/>
     </row>
     <row r="220" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B220" s="6"/>
+      <c r="P220" s="6"/>
+      <c r="Q220" s="6"/>
+    </row>
+    <row r="221" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P221" s="6"/>
+      <c r="Q221" s="6"/>
+    </row>
+    <row r="222" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P222" s="6"/>
+      <c r="Q222" s="6"/>
+    </row>
+    <row r="223" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P223" s="6"/>
+      <c r="Q223" s="6"/>
+    </row>
+    <row r="224" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="P224" s="6"/>
+      <c r="Q224" s="6"/>
+    </row>
+    <row r="225" spans="16:16" x14ac:dyDescent="0.3">
+      <c r="P225" s="6"/>
     </row>
   </sheetData>
   <mergeCells count="4">
@@ -30152,7 +30391,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C76" sqref="C76"/>
+      <selection pane="bottomLeft" activeCell="A76" sqref="A76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -30179,34 +30418,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.3">
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="30"/>
-      <c r="D1" s="30"/>
-      <c r="E1" s="30"/>
-      <c r="F1" s="30"/>
-      <c r="G1" s="30"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="30" t="s">
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="30"/>
+      <c r="I1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="30"/>
-      <c r="K1" s="30"/>
-      <c r="L1" s="30"/>
-      <c r="M1" s="30"/>
-      <c r="N1" s="30"/>
-      <c r="O1" s="31"/>
-      <c r="P1" s="29" t="s">
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="30"/>
+      <c r="P1" s="28" t="s">
         <v>2</v>
       </c>
-      <c r="Q1" s="30"/>
-      <c r="R1" s="30"/>
-      <c r="S1" s="29" t="s">
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="T1" s="30"/>
-      <c r="U1" s="31"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="30"/>
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
@@ -31786,7 +32025,7 @@
         <v>8328</v>
       </c>
       <c r="R23" s="8">
-        <f t="shared" ref="R23:R68" si="9">Q23/P23</f>
+        <f t="shared" ref="R23:R70" si="9">Q23/P23</f>
         <v>1189.7142857142858</v>
       </c>
       <c r="S23" s="6">
@@ -33922,15 +34161,15 @@
         <v>1798</v>
       </c>
       <c r="M53" s="6">
-        <f t="shared" ref="M53:M68" si="20">J53/I53</f>
+        <f t="shared" ref="M53:M70" si="20">J53/I53</f>
         <v>5209.375</v>
       </c>
       <c r="N53" s="6">
-        <f t="shared" ref="N53:N68" si="21">K53/I53</f>
+        <f t="shared" ref="N53:N70" si="21">K53/I53</f>
         <v>1070.75</v>
       </c>
       <c r="O53" s="8">
-        <f t="shared" ref="O53:O68" si="22">L53/I53</f>
+        <f t="shared" ref="O53:O70" si="22">L53/I53</f>
         <v>224.75</v>
       </c>
       <c r="P53" s="6">
@@ -34626,15 +34865,15 @@
         <v>681</v>
       </c>
       <c r="F63" s="6">
-        <f t="shared" ref="F63:F68" si="27">C63/B63</f>
+        <f t="shared" ref="F63:F70" si="27">C63/B63</f>
         <v>40.142857142857146</v>
       </c>
       <c r="G63" s="6">
-        <f t="shared" ref="G63:G68" si="28">D63/B63</f>
+        <f t="shared" ref="G63:G70" si="28">D63/B63</f>
         <v>39.285714285714285</v>
       </c>
       <c r="H63" s="8">
-        <f t="shared" ref="H63:H68" si="29">E63/B63</f>
+        <f t="shared" ref="H63:H70" si="29">E63/B63</f>
         <v>97.285714285714292</v>
       </c>
       <c r="I63" s="6">
@@ -35051,31 +35290,127 @@
       <c r="A69" s="9">
         <v>45368</v>
       </c>
-      <c r="B69" s="6"/>
-      <c r="C69" s="6"/>
-      <c r="D69" s="6"/>
-      <c r="E69" s="6"/>
-      <c r="I69" s="6"/>
-      <c r="J69" s="6"/>
-      <c r="K69" s="6"/>
-      <c r="L69" s="6"/>
-      <c r="P69" s="6"/>
-      <c r="Q69" s="6"/>
+      <c r="B69" s="6">
+        <v>9</v>
+      </c>
+      <c r="C69" s="6">
+        <v>1490</v>
+      </c>
+      <c r="D69" s="6">
+        <v>471</v>
+      </c>
+      <c r="E69" s="6">
+        <v>1501</v>
+      </c>
+      <c r="F69" s="6">
+        <f t="shared" si="27"/>
+        <v>165.55555555555554</v>
+      </c>
+      <c r="G69" s="6">
+        <f t="shared" si="28"/>
+        <v>52.333333333333336</v>
+      </c>
+      <c r="H69" s="8">
+        <f t="shared" si="29"/>
+        <v>166.77777777777777</v>
+      </c>
+      <c r="I69" s="6">
+        <v>11</v>
+      </c>
+      <c r="J69" s="6">
+        <v>22003</v>
+      </c>
+      <c r="K69" s="6">
+        <v>2973</v>
+      </c>
+      <c r="L69" s="6">
+        <v>1390</v>
+      </c>
+      <c r="M69" s="6">
+        <f t="shared" si="20"/>
+        <v>2000.2727272727273</v>
+      </c>
+      <c r="N69" s="6">
+        <f t="shared" si="21"/>
+        <v>270.27272727272725</v>
+      </c>
+      <c r="O69" s="8">
+        <f t="shared" si="22"/>
+        <v>126.36363636363636</v>
+      </c>
+      <c r="P69" s="6">
+        <v>6</v>
+      </c>
+      <c r="Q69" s="6">
+        <v>9174</v>
+      </c>
+      <c r="R69" s="8">
+        <f t="shared" si="9"/>
+        <v>1529</v>
+      </c>
     </row>
     <row r="70" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A70" s="9">
         <v>45369</v>
       </c>
-      <c r="B70" s="6"/>
-      <c r="C70" s="6"/>
-      <c r="D70" s="6"/>
-      <c r="E70" s="6"/>
-      <c r="I70" s="6"/>
-      <c r="J70" s="6"/>
-      <c r="K70" s="6"/>
-      <c r="L70" s="6"/>
-      <c r="P70" s="6"/>
-      <c r="Q70" s="6"/>
+      <c r="B70" s="6">
+        <v>8</v>
+      </c>
+      <c r="C70" s="6">
+        <v>323</v>
+      </c>
+      <c r="D70" s="6">
+        <v>426</v>
+      </c>
+      <c r="E70" s="6">
+        <v>821</v>
+      </c>
+      <c r="F70" s="6">
+        <f t="shared" si="27"/>
+        <v>40.375</v>
+      </c>
+      <c r="G70" s="6">
+        <f t="shared" si="28"/>
+        <v>53.25</v>
+      </c>
+      <c r="H70" s="8">
+        <f t="shared" si="29"/>
+        <v>102.625</v>
+      </c>
+      <c r="I70" s="6">
+        <v>11</v>
+      </c>
+      <c r="J70" s="6">
+        <v>23471</v>
+      </c>
+      <c r="K70" s="6">
+        <v>5692</v>
+      </c>
+      <c r="L70" s="6">
+        <v>1317</v>
+      </c>
+      <c r="M70" s="6">
+        <f t="shared" si="20"/>
+        <v>2133.7272727272725</v>
+      </c>
+      <c r="N70" s="6">
+        <f t="shared" si="21"/>
+        <v>517.4545454545455</v>
+      </c>
+      <c r="O70" s="8">
+        <f t="shared" si="22"/>
+        <v>119.72727272727273</v>
+      </c>
+      <c r="P70" s="6">
+        <v>5</v>
+      </c>
+      <c r="Q70" s="6">
+        <v>15345</v>
+      </c>
+      <c r="R70" s="8">
+        <f t="shared" si="9"/>
+        <v>3069</v>
+      </c>
     </row>
     <row r="71" spans="1:21" x14ac:dyDescent="0.3">
       <c r="B71" s="6"/>
@@ -35114,6 +35449,7 @@
       <c r="Q73" s="6"/>
     </row>
     <row r="74" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B74" s="6"/>
       <c r="C74" s="6"/>
       <c r="D74" s="6"/>
       <c r="E74" s="6"/>
@@ -35311,6 +35647,9 @@
     </row>
     <row r="91" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I91" s="6"/>
+      <c r="J91" s="6"/>
+      <c r="K91" s="6"/>
+      <c r="L91" s="6"/>
     </row>
     <row r="92" spans="2:17" x14ac:dyDescent="0.3">
       <c r="I92" s="6"/>
@@ -35423,485 +35762,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346A044C-6F3E-436F-84AC-DB98BA731517}">
-  <dimension ref="A2:M22"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
-  <cols>
-    <col min="3" max="3" width="12.44140625" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" t="s">
-        <v>16</v>
-      </c>
-      <c r="G2" t="s">
-        <v>83</v>
-      </c>
-      <c r="H2" t="s">
-        <v>18</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" t="s">
-        <v>26</v>
-      </c>
-      <c r="M2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B3">
-        <v>919</v>
-      </c>
-      <c r="C3">
-        <v>681403</v>
-      </c>
-      <c r="D3">
-        <v>1230276</v>
-      </c>
-      <c r="E3">
-        <v>3481884</v>
-      </c>
-      <c r="F3">
-        <v>1248</v>
-      </c>
-      <c r="G3">
-        <v>7505763</v>
-      </c>
-      <c r="H3">
-        <v>931280</v>
-      </c>
-      <c r="I3">
-        <v>707847</v>
-      </c>
-      <c r="J3">
-        <v>923</v>
-      </c>
-      <c r="K3">
-        <v>4848438</v>
-      </c>
-      <c r="L3">
-        <v>349</v>
-      </c>
-      <c r="M3">
-        <v>10688244</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="C4">
-        <v>510</v>
-      </c>
-      <c r="D4">
-        <v>1500</v>
-      </c>
-      <c r="E4">
-        <v>4100</v>
-      </c>
-      <c r="G4">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>9500</v>
-      </c>
-      <c r="I4">
-        <v>1279</v>
-      </c>
-      <c r="K4">
-        <v>0</v>
-      </c>
-      <c r="M4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>55</v>
-      </c>
-      <c r="C5">
-        <v>13151</v>
-      </c>
-      <c r="D5">
-        <v>25456</v>
-      </c>
-      <c r="E5">
-        <v>81468</v>
-      </c>
-      <c r="G5">
-        <v>187100</v>
-      </c>
-      <c r="H5">
-        <v>24800</v>
-      </c>
-      <c r="I5">
-        <v>25926</v>
-      </c>
-      <c r="K5">
-        <v>161665</v>
-      </c>
-      <c r="M5">
-        <v>847671</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>56</v>
-      </c>
-      <c r="C6">
-        <v>4635.3945578231296</v>
-      </c>
-      <c r="D6">
-        <v>8369.224489795919</v>
-      </c>
-      <c r="E6">
-        <v>23686.285714285714</v>
-      </c>
-      <c r="G6">
-        <v>51059.612244897959</v>
-      </c>
-      <c r="H6">
-        <v>6335.2380952380954</v>
-      </c>
-      <c r="I6">
-        <v>4815.2857142857147</v>
-      </c>
-      <c r="K6">
-        <v>32982.571428571428</v>
-      </c>
-      <c r="M6">
-        <v>72709.142857142855</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>57</v>
-      </c>
-      <c r="C7">
-        <v>3917</v>
-      </c>
-      <c r="D7">
-        <v>7700</v>
-      </c>
-      <c r="E7">
-        <v>22100</v>
-      </c>
-      <c r="G7">
-        <v>38400</v>
-      </c>
-      <c r="H7">
-        <v>5474</v>
-      </c>
-      <c r="I7">
-        <v>4422</v>
-      </c>
-      <c r="K7">
-        <v>28016</v>
-      </c>
-      <c r="M7">
-        <v>18395</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8">
-        <v>2623.895375038468</v>
-      </c>
-      <c r="D8">
-        <v>3842.9305202547876</v>
-      </c>
-      <c r="E8">
-        <v>11596.721585614037</v>
-      </c>
-      <c r="G8">
-        <v>37255.368355915067</v>
-      </c>
-      <c r="H8">
-        <v>4025.0868370337184</v>
-      </c>
-      <c r="I8">
-        <v>2682.5965238158797</v>
-      </c>
-      <c r="K8">
-        <v>22670.2202970123</v>
-      </c>
-      <c r="M8">
-        <v>131648.55887015644</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="B10" t="s">
-        <v>84</v>
-      </c>
-      <c r="C10" t="s">
-        <v>54</v>
-      </c>
-      <c r="D10" t="s">
-        <v>55</v>
-      </c>
-      <c r="E10" t="s">
-        <v>56</v>
-      </c>
-      <c r="F10" t="s">
-        <v>57</v>
-      </c>
-      <c r="G10" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>82</v>
-      </c>
-      <c r="B11">
-        <v>919</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12">
-        <v>681403</v>
-      </c>
-      <c r="C12">
-        <v>510</v>
-      </c>
-      <c r="D12">
-        <v>13151</v>
-      </c>
-      <c r="E12">
-        <v>4635.3945578231296</v>
-      </c>
-      <c r="F12">
-        <v>3917</v>
-      </c>
-      <c r="G12">
-        <v>2623.895375038468</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>30</v>
-      </c>
-      <c r="B13">
-        <v>1230276</v>
-      </c>
-      <c r="C13">
-        <v>1500</v>
-      </c>
-      <c r="D13">
-        <v>25456</v>
-      </c>
-      <c r="E13">
-        <v>8369.224489795919</v>
-      </c>
-      <c r="F13">
-        <v>7700</v>
-      </c>
-      <c r="G13">
-        <v>3842.9305202547876</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14">
-        <v>3481884</v>
-      </c>
-      <c r="C14">
-        <v>4100</v>
-      </c>
-      <c r="D14">
-        <v>81468</v>
-      </c>
-      <c r="E14">
-        <v>23686.285714285714</v>
-      </c>
-      <c r="F14">
-        <v>22100</v>
-      </c>
-      <c r="G14">
-        <v>11596.721585614037</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>16</v>
-      </c>
-      <c r="B15">
-        <v>1248</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>83</v>
-      </c>
-      <c r="B16">
-        <v>7505763</v>
-      </c>
-      <c r="C16">
-        <v>2</v>
-      </c>
-      <c r="D16">
-        <v>187100</v>
-      </c>
-      <c r="E16">
-        <v>51059.612244897959</v>
-      </c>
-      <c r="F16">
-        <v>38400</v>
-      </c>
-      <c r="G16">
-        <v>37255.368355915067</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17">
-        <v>931280</v>
-      </c>
-      <c r="C17">
-        <v>9500</v>
-      </c>
-      <c r="D17">
-        <v>24800</v>
-      </c>
-      <c r="E17">
-        <v>6335.2380952380954</v>
-      </c>
-      <c r="F17">
-        <v>5474</v>
-      </c>
-      <c r="G17">
-        <v>4025.0868370337184</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>19</v>
-      </c>
-      <c r="B18">
-        <v>707847</v>
-      </c>
-      <c r="C18">
-        <v>1279</v>
-      </c>
-      <c r="D18">
-        <v>25926</v>
-      </c>
-      <c r="E18">
-        <v>4815.2857142857147</v>
-      </c>
-      <c r="F18">
-        <v>4422</v>
-      </c>
-      <c r="G18">
-        <v>2682.5965238158797</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>23</v>
-      </c>
-      <c r="B19">
-        <v>923</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>24</v>
-      </c>
-      <c r="B20">
-        <v>4848438</v>
-      </c>
-      <c r="C20">
-        <v>0</v>
-      </c>
-      <c r="D20">
-        <v>161665</v>
-      </c>
-      <c r="E20">
-        <v>32982.571428571428</v>
-      </c>
-      <c r="F20">
-        <v>28016</v>
-      </c>
-      <c r="G20">
-        <v>22670.2202970123</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
-        <v>349</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22">
-        <v>10688244</v>
-      </c>
-      <c r="C22">
-        <v>0</v>
-      </c>
-      <c r="D22">
-        <v>847671</v>
-      </c>
-      <c r="E22">
-        <v>72709.142857142855</v>
-      </c>
-      <c r="F22">
-        <v>18395</v>
-      </c>
-      <c r="G22">
-        <v>131648.55887015644</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6AAE58A-8A5A-4C93-AE14-DE5004288388}">
   <dimension ref="A1:F4"/>
   <sheetViews>
@@ -35960,7 +35820,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E62C3539-067A-49FB-A3DE-0B279692F912}">
   <dimension ref="A1:T42"/>
   <sheetViews>
@@ -37629,7 +37489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC47CE33-EEC3-446C-940D-05592E4B50CB}">
   <dimension ref="A1:N8"/>
   <sheetViews>
@@ -37640,24 +37500,24 @@
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="A1" s="32" t="s">
+      <c r="A1" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="32"/>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="F1" s="32" t="s">
+      <c r="B1" s="31"/>
+      <c r="C1" s="31"/>
+      <c r="D1" s="31"/>
+      <c r="F1" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="G1" s="32"/>
-      <c r="H1" s="32"/>
-      <c r="I1" s="32"/>
-      <c r="K1" s="32" t="s">
+      <c r="G1" s="31"/>
+      <c r="H1" s="31"/>
+      <c r="I1" s="31"/>
+      <c r="K1" s="31" t="s">
         <v>63</v>
       </c>
-      <c r="L1" s="32"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
+      <c r="L1" s="31"/>
+      <c r="M1" s="31"/>
+      <c r="N1" s="31"/>
     </row>
     <row r="2" spans="1:14" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
@@ -37941,7 +37801,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6748DF8D-1E96-42F5-BE18-DD686141E658}">
   <dimension ref="B2:M9"/>
   <sheetViews>
@@ -38063,4 +37923,483 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{346A044C-6F3E-436F-84AC-DB98BA731517}">
+  <dimension ref="A2:M22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="12.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B2" t="s">
+        <v>82</v>
+      </c>
+      <c r="C2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" t="s">
+        <v>83</v>
+      </c>
+      <c r="H2" t="s">
+        <v>18</v>
+      </c>
+      <c r="I2" t="s">
+        <v>19</v>
+      </c>
+      <c r="J2" t="s">
+        <v>23</v>
+      </c>
+      <c r="K2" t="s">
+        <v>24</v>
+      </c>
+      <c r="L2" t="s">
+        <v>26</v>
+      </c>
+      <c r="M2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B3">
+        <v>919</v>
+      </c>
+      <c r="C3">
+        <v>681403</v>
+      </c>
+      <c r="D3">
+        <v>1230276</v>
+      </c>
+      <c r="E3">
+        <v>3481884</v>
+      </c>
+      <c r="F3">
+        <v>1248</v>
+      </c>
+      <c r="G3">
+        <v>7505763</v>
+      </c>
+      <c r="H3">
+        <v>931280</v>
+      </c>
+      <c r="I3">
+        <v>707847</v>
+      </c>
+      <c r="J3">
+        <v>923</v>
+      </c>
+      <c r="K3">
+        <v>4848438</v>
+      </c>
+      <c r="L3">
+        <v>349</v>
+      </c>
+      <c r="M3">
+        <v>10688244</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>54</v>
+      </c>
+      <c r="C4">
+        <v>510</v>
+      </c>
+      <c r="D4">
+        <v>1500</v>
+      </c>
+      <c r="E4">
+        <v>4100</v>
+      </c>
+      <c r="G4">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>9500</v>
+      </c>
+      <c r="I4">
+        <v>1279</v>
+      </c>
+      <c r="K4">
+        <v>0</v>
+      </c>
+      <c r="M4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>55</v>
+      </c>
+      <c r="C5">
+        <v>13151</v>
+      </c>
+      <c r="D5">
+        <v>25456</v>
+      </c>
+      <c r="E5">
+        <v>81468</v>
+      </c>
+      <c r="G5">
+        <v>187100</v>
+      </c>
+      <c r="H5">
+        <v>24800</v>
+      </c>
+      <c r="I5">
+        <v>25926</v>
+      </c>
+      <c r="K5">
+        <v>161665</v>
+      </c>
+      <c r="M5">
+        <v>847671</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>56</v>
+      </c>
+      <c r="C6">
+        <v>4635.3945578231296</v>
+      </c>
+      <c r="D6">
+        <v>8369.224489795919</v>
+      </c>
+      <c r="E6">
+        <v>23686.285714285714</v>
+      </c>
+      <c r="G6">
+        <v>51059.612244897959</v>
+      </c>
+      <c r="H6">
+        <v>6335.2380952380954</v>
+      </c>
+      <c r="I6">
+        <v>4815.2857142857147</v>
+      </c>
+      <c r="K6">
+        <v>32982.571428571428</v>
+      </c>
+      <c r="M6">
+        <v>72709.142857142855</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>57</v>
+      </c>
+      <c r="C7">
+        <v>3917</v>
+      </c>
+      <c r="D7">
+        <v>7700</v>
+      </c>
+      <c r="E7">
+        <v>22100</v>
+      </c>
+      <c r="G7">
+        <v>38400</v>
+      </c>
+      <c r="H7">
+        <v>5474</v>
+      </c>
+      <c r="I7">
+        <v>4422</v>
+      </c>
+      <c r="K7">
+        <v>28016</v>
+      </c>
+      <c r="M7">
+        <v>18395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>58</v>
+      </c>
+      <c r="C8">
+        <v>2623.895375038468</v>
+      </c>
+      <c r="D8">
+        <v>3842.9305202547876</v>
+      </c>
+      <c r="E8">
+        <v>11596.721585614037</v>
+      </c>
+      <c r="G8">
+        <v>37255.368355915067</v>
+      </c>
+      <c r="H8">
+        <v>4025.0868370337184</v>
+      </c>
+      <c r="I8">
+        <v>2682.5965238158797</v>
+      </c>
+      <c r="K8">
+        <v>22670.2202970123</v>
+      </c>
+      <c r="M8">
+        <v>131648.55887015644</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" t="s">
+        <v>56</v>
+      </c>
+      <c r="F10" t="s">
+        <v>57</v>
+      </c>
+      <c r="G10" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11">
+        <v>919</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>681403</v>
+      </c>
+      <c r="C12">
+        <v>510</v>
+      </c>
+      <c r="D12">
+        <v>13151</v>
+      </c>
+      <c r="E12">
+        <v>4635.3945578231296</v>
+      </c>
+      <c r="F12">
+        <v>3917</v>
+      </c>
+      <c r="G12">
+        <v>2623.895375038468</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>30</v>
+      </c>
+      <c r="B13">
+        <v>1230276</v>
+      </c>
+      <c r="C13">
+        <v>1500</v>
+      </c>
+      <c r="D13">
+        <v>25456</v>
+      </c>
+      <c r="E13">
+        <v>8369.224489795919</v>
+      </c>
+      <c r="F13">
+        <v>7700</v>
+      </c>
+      <c r="G13">
+        <v>3842.9305202547876</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>3481884</v>
+      </c>
+      <c r="C14">
+        <v>4100</v>
+      </c>
+      <c r="D14">
+        <v>81468</v>
+      </c>
+      <c r="E14">
+        <v>23686.285714285714</v>
+      </c>
+      <c r="F14">
+        <v>22100</v>
+      </c>
+      <c r="G14">
+        <v>11596.721585614037</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15">
+        <v>1248</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>83</v>
+      </c>
+      <c r="B16">
+        <v>7505763</v>
+      </c>
+      <c r="C16">
+        <v>2</v>
+      </c>
+      <c r="D16">
+        <v>187100</v>
+      </c>
+      <c r="E16">
+        <v>51059.612244897959</v>
+      </c>
+      <c r="F16">
+        <v>38400</v>
+      </c>
+      <c r="G16">
+        <v>37255.368355915067</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17">
+        <v>931280</v>
+      </c>
+      <c r="C17">
+        <v>9500</v>
+      </c>
+      <c r="D17">
+        <v>24800</v>
+      </c>
+      <c r="E17">
+        <v>6335.2380952380954</v>
+      </c>
+      <c r="F17">
+        <v>5474</v>
+      </c>
+      <c r="G17">
+        <v>4025.0868370337184</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18">
+        <v>707847</v>
+      </c>
+      <c r="C18">
+        <v>1279</v>
+      </c>
+      <c r="D18">
+        <v>25926</v>
+      </c>
+      <c r="E18">
+        <v>4815.2857142857147</v>
+      </c>
+      <c r="F18">
+        <v>4422</v>
+      </c>
+      <c r="G18">
+        <v>2682.5965238158797</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19">
+        <v>923</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20">
+        <v>4848438</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>161665</v>
+      </c>
+      <c r="E20">
+        <v>32982.571428571428</v>
+      </c>
+      <c r="F20">
+        <v>28016</v>
+      </c>
+      <c r="G20">
+        <v>22670.2202970123</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B21">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22">
+        <v>10688244</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>847671</v>
+      </c>
+      <c r="E22">
+        <v>72709.142857142855</v>
+      </c>
+      <c r="F22">
+        <v>18395</v>
+      </c>
+      <c r="G22">
+        <v>131648.55887015644</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>